<commit_message>
Added features to APOIV
</commit_message>
<xml_diff>
--- a/tabular/virus/flavi-reference_feature_locations.xlsx
+++ b/tabular/virus/flavi-reference_feature_locations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1620" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="115">
   <si>
     <t>featureName</t>
   </si>
@@ -576,9 +576,69 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2283">
+  <cellStyleXfs count="2343">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2926,7 +2986,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2283">
+  <cellStyles count="2343">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -4069,6 +4129,36 @@
     <cellStyle name="Followed Hyperlink" xfId="2278" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2280" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2342" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -5209,6 +5299,36 @@
     <cellStyle name="Hyperlink" xfId="2277" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2279" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2341" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5546,10 +5666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1471"/>
+  <dimension ref="A1:H1485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G150" sqref="A1:G155"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6910,7 +7030,7 @@
       <c r="D59" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E59" s="7" t="s">
         <v>83</v>
       </c>
       <c r="F59" s="9">
@@ -6933,7 +7053,7 @@
       <c r="D60" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E60" s="7" t="s">
         <v>70</v>
       </c>
       <c r="F60" s="9">
@@ -6945,373 +7065,374 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="37" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C61" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F61" s="1">
+      <c r="D61" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F61" s="9">
         <v>1</v>
       </c>
-      <c r="G61" s="1">
-        <v>10242</v>
+      <c r="G61" s="9">
+        <v>2268</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F62" s="9">
+        <v>1</v>
+      </c>
+      <c r="G62" s="9">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F63" s="9">
+        <v>331</v>
+      </c>
+      <c r="G63" s="9">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F64" s="9">
+        <v>589</v>
+      </c>
+      <c r="G64" s="9">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B65" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F65" s="9">
+        <v>814</v>
+      </c>
+      <c r="G65" s="9">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B66" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" s="9">
+        <v>2269</v>
+      </c>
+      <c r="G66" s="9">
+        <v>3327</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C67" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F67" s="9">
+        <v>3328</v>
+      </c>
+      <c r="G67" s="9">
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B68" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F68" s="9">
+        <v>4003</v>
+      </c>
+      <c r="G68" s="9">
+        <v>4392</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C69" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="9">
+        <v>4393</v>
+      </c>
+      <c r="G69" s="9">
+        <v>6240</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B70" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C70" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F70" s="9">
+        <v>6241</v>
+      </c>
+      <c r="G70" s="9">
+        <v>6597</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C71" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" s="9">
+        <v>6598</v>
+      </c>
+      <c r="G71" s="9">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B72" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F72" s="9">
+        <v>6667</v>
+      </c>
+      <c r="G72" s="9">
+        <v>7422</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C73" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="9">
+        <v>7423</v>
+      </c>
+      <c r="G73" s="9">
+        <v>10113</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C74" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F74" s="9">
+        <v>2269</v>
+      </c>
+      <c r="G74" s="9">
+        <v>10116</v>
+      </c>
+      <c r="H74" s="27"/>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B62" s="37" t="s">
+      <c r="B75" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D62" s="24" t="s">
+      <c r="C75" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E75" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F75" s="1">
+        <v>1</v>
+      </c>
+      <c r="G75" s="1">
+        <v>10242</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B76" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C76" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E76" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F76" s="1">
         <v>1</v>
       </c>
-      <c r="G62" s="1">
+      <c r="G76" s="1">
         <v>10242</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B63" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C63" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E63" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F63" s="27">
-        <v>1</v>
-      </c>
-      <c r="G63" s="27">
-        <v>10839</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B64" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C64" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E64" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F64" s="27">
-        <v>1</v>
-      </c>
-      <c r="G64" s="27">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C65" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D65" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E65" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F65" s="27">
-        <v>112</v>
-      </c>
-      <c r="G65" s="27">
-        <v>10359</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B66" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C66" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D66" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E66" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F66" s="27">
-        <v>112</v>
-      </c>
-      <c r="G66" s="27">
-        <v>2436</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B67" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C67" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D67" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E67" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="F67" s="27">
-        <v>112</v>
-      </c>
-      <c r="G67" s="27">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B68" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C68" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D68" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E68" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="F68" s="27">
-        <v>442</v>
-      </c>
-      <c r="G68" s="27">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B69" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C69" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E69" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F69" s="27">
-        <v>946</v>
-      </c>
-      <c r="G69" s="27">
-        <v>2436</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B70" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C70" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D70" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E70" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="F70" s="27">
-        <v>2437</v>
-      </c>
-      <c r="G70" s="27">
-        <v>10356</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B71" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C71" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D71" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E71" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="F71" s="27">
-        <v>2437</v>
-      </c>
-      <c r="G71" s="27">
-        <v>3495</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B72" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C72" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D72" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E72" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="F72" s="27">
-        <v>3496</v>
-      </c>
-      <c r="G72" s="27">
-        <v>4185</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B73" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C73" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D73" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E73" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="F73" s="27">
-        <v>4186</v>
-      </c>
-      <c r="G73" s="27">
-        <v>4578</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B74" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C74" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D74" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E74" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F74" s="27">
-        <v>4579</v>
-      </c>
-      <c r="G74" s="27">
-        <v>6444</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B75" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C75" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D75" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E75" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="F75" s="27">
-        <v>6445</v>
-      </c>
-      <c r="G75" s="27">
-        <v>6822</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B76" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C76" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D76" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E76" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F76" s="27">
-        <v>6823</v>
-      </c>
-      <c r="G76" s="27">
-        <v>6891</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:8">
       <c r="A77" s="36" t="s">
         <v>33</v>
       </c>
@@ -7325,16 +7446,16 @@
         <v>43</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F77" s="27">
-        <v>6892</v>
+        <v>1</v>
       </c>
       <c r="G77" s="27">
-        <v>7647</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+        <v>10839</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" s="36" t="s">
         <v>33</v>
       </c>
@@ -7348,16 +7469,16 @@
         <v>43</v>
       </c>
       <c r="E78" s="27" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F78" s="27">
-        <v>7648</v>
+        <v>1</v>
       </c>
       <c r="G78" s="27">
-        <v>10356</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" s="36" t="s">
         <v>33</v>
       </c>
@@ -7371,335 +7492,335 @@
         <v>43</v>
       </c>
       <c r="E79" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F79" s="27">
+        <v>112</v>
+      </c>
+      <c r="G79" s="27">
+        <v>10359</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B80" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C80" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E80" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F80" s="27">
+        <v>112</v>
+      </c>
+      <c r="G80" s="27">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B81" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C81" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E81" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F81" s="27">
+        <v>112</v>
+      </c>
+      <c r="G81" s="27">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B82" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C82" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E82" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F82" s="27">
+        <v>442</v>
+      </c>
+      <c r="G82" s="27">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B83" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C83" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E83" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F83" s="27">
+        <v>946</v>
+      </c>
+      <c r="G83" s="27">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B84" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C84" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F84" s="27">
+        <v>2437</v>
+      </c>
+      <c r="G84" s="27">
+        <v>10356</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B85" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C85" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E85" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" s="27">
+        <v>2437</v>
+      </c>
+      <c r="G85" s="27">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B86" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C86" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E86" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="F86" s="27">
+        <v>3496</v>
+      </c>
+      <c r="G86" s="27">
+        <v>4185</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B87" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C87" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E87" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="F87" s="27">
+        <v>4186</v>
+      </c>
+      <c r="G87" s="27">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B88" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C88" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E88" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F88" s="27">
+        <v>4579</v>
+      </c>
+      <c r="G88" s="27">
+        <v>6444</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B89" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C89" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E89" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F89" s="27">
+        <v>6445</v>
+      </c>
+      <c r="G89" s="27">
+        <v>6822</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B90" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C90" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E90" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" s="27">
+        <v>6823</v>
+      </c>
+      <c r="G90" s="27">
+        <v>6891</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B91" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C91" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E91" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F91" s="27">
+        <v>6892</v>
+      </c>
+      <c r="G91" s="27">
+        <v>7647</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C92" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E92" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F92" s="27">
+        <v>7648</v>
+      </c>
+      <c r="G92" s="27">
+        <v>10356</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B93" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C93" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E93" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F79" s="27">
+      <c r="F93" s="27">
         <v>10357</v>
       </c>
-      <c r="G79" s="27">
+      <c r="G93" s="27">
         <v>10839</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B80" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C80" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D80" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E80" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F80" s="27">
-        <v>1</v>
-      </c>
-      <c r="G80" s="27">
-        <v>9646</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B81" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C81" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D81" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E81" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F81" s="27">
-        <v>1</v>
-      </c>
-      <c r="G81" s="27">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B82" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C82" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D82" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E82" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F82" s="27">
-        <v>342</v>
-      </c>
-      <c r="G82" s="27">
-        <v>9377</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="A83" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B83" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C83" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D83" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E83" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F83" s="27">
-        <v>342</v>
-      </c>
-      <c r="G83" s="27">
-        <v>2579</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B84" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C84" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D84" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E84" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="F84" s="27">
-        <v>342</v>
-      </c>
-      <c r="G84" s="27">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B85" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C85" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D85" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E85" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="F85" s="27">
-        <v>915</v>
-      </c>
-      <c r="G85" s="27">
-        <v>1490</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B86" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C86" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D86" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E86" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="F86" s="27">
-        <v>1491</v>
-      </c>
-      <c r="G86" s="27">
-        <v>2579</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B87" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C87" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D87" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E87" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="F87" s="27">
-        <v>2580</v>
-      </c>
-      <c r="G87" s="27">
-        <v>9374</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B88" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C88" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D88" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E88" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F88" s="27">
-        <v>2580</v>
-      </c>
-      <c r="G88" s="27">
-        <v>2768</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B89" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C89" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D89" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E89" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="F89" s="27">
-        <v>2769</v>
-      </c>
-      <c r="G89" s="27">
-        <v>3419</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="A90" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B90" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C90" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D90" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E90" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F90" s="27">
-        <v>3420</v>
-      </c>
-      <c r="G90" s="27">
-        <v>5312</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="A91" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B91" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C91" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D91" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E91" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="F91" s="27">
-        <v>5313</v>
-      </c>
-      <c r="G91" s="27">
-        <v>5474</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B92" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C92" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D92" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E92" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="F92" s="27">
-        <v>5475</v>
-      </c>
-      <c r="G92" s="27">
-        <v>6257</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B93" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C93" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D93" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E93" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F93" s="27">
-        <v>6258</v>
-      </c>
-      <c r="G93" s="27">
-        <v>7601</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -7716,13 +7837,13 @@
         <v>107</v>
       </c>
       <c r="E94" s="27" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="F94" s="27">
-        <v>7602</v>
+        <v>1</v>
       </c>
       <c r="G94" s="27">
-        <v>9374</v>
+        <v>9646</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -7739,307 +7860,333 @@
         <v>107</v>
       </c>
       <c r="E95" s="27" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F95" s="27">
-        <v>9378</v>
+        <v>1</v>
       </c>
       <c r="G95" s="27">
-        <v>9646</v>
+        <v>341</v>
       </c>
     </row>
     <row r="96" spans="1:7">
-      <c r="A96" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B96" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C96" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D96"/>
+      <c r="A96" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B96" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C96" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D96" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E96" s="27" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="F96" s="27">
-        <v>1</v>
+        <v>342</v>
       </c>
       <c r="G96" s="27">
-        <v>9867</v>
+        <v>9377</v>
       </c>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B97" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C97" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D97"/>
+      <c r="A97" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B97" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C97" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D97" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E97" s="27" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="F97" s="27">
-        <v>1</v>
+        <v>342</v>
       </c>
       <c r="G97" s="27">
-        <v>327</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="98" spans="1:7">
-      <c r="A98" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B98" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C98" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D98"/>
+      <c r="A98" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B98" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C98" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D98" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E98" s="27" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="F98" s="27">
-        <v>328</v>
+        <v>342</v>
       </c>
       <c r="G98" s="27">
-        <v>9501</v>
+        <v>914</v>
       </c>
     </row>
     <row r="99" spans="1:7">
-      <c r="A99" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B99" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C99" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D99"/>
+      <c r="A99" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B99" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C99" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E99" s="27" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F99" s="27">
-        <v>328</v>
+        <v>915</v>
       </c>
       <c r="G99" s="27">
-        <v>2199</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="100" spans="1:7">
-      <c r="A100" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B100" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C100" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D100"/>
+      <c r="A100" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B100" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C100" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D100" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E100" s="27" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="F100" s="27">
-        <v>328</v>
+        <v>1491</v>
       </c>
       <c r="G100" s="27">
-        <v>564</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="101" spans="1:7">
-      <c r="A101" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B101" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C101" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D101"/>
+      <c r="A101" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B101" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C101" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E101" s="27" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F101" s="27">
-        <v>565</v>
+        <v>2580</v>
       </c>
       <c r="G101" s="27">
-        <v>1137</v>
+        <v>9374</v>
       </c>
     </row>
     <row r="102" spans="1:7">
-      <c r="A102" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B102" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C102" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D102"/>
+      <c r="A102" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B102" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C102" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D102" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E102" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F102" s="27">
-        <v>1138</v>
+        <v>2580</v>
       </c>
       <c r="G102" s="27">
-        <v>2199</v>
+        <v>2768</v>
       </c>
     </row>
     <row r="103" spans="1:7">
-      <c r="A103" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B103" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C103" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D103"/>
+      <c r="A103" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B103" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C103" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D103" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E103" s="27" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="F103" s="27">
-        <v>2200</v>
+        <v>2769</v>
       </c>
       <c r="G103" s="27">
-        <v>2910</v>
+        <v>3419</v>
       </c>
     </row>
     <row r="104" spans="1:7">
-      <c r="A104" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B104" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C104" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D104"/>
+      <c r="A104" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B104" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C104" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D104" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E104" s="27" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="F104" s="27">
-        <v>2911</v>
+        <v>3420</v>
       </c>
       <c r="G104" s="27">
-        <v>9498</v>
+        <v>5312</v>
       </c>
     </row>
     <row r="105" spans="1:7">
-      <c r="A105" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B105" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C105" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D105"/>
+      <c r="A105" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B105" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C105" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D105" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E105" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F105" s="27">
-        <v>2911</v>
+        <v>5313</v>
       </c>
       <c r="G105" s="27">
-        <v>3630</v>
+        <v>5474</v>
       </c>
     </row>
     <row r="106" spans="1:7">
-      <c r="A106" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B106" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C106" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D106"/>
+      <c r="A106" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B106" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C106" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D106" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E106" s="27" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="F106" s="27">
-        <v>3631</v>
+        <v>5475</v>
       </c>
       <c r="G106" s="27">
-        <v>5514</v>
+        <v>6257</v>
       </c>
     </row>
     <row r="107" spans="1:7">
-      <c r="A107" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B107" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C107" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D107"/>
+      <c r="A107" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B107" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C107" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D107" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E107" s="27" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="F107" s="27">
-        <v>5515</v>
+        <v>6258</v>
       </c>
       <c r="G107" s="27">
-        <v>5637</v>
+        <v>7601</v>
       </c>
     </row>
     <row r="108" spans="1:7">
-      <c r="A108" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B108" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C108" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D108"/>
+      <c r="A108" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B108" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C108" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D108" s="40" t="s">
+        <v>107</v>
+      </c>
       <c r="E108" s="27" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="F108" s="27">
-        <v>5638</v>
+        <v>7602</v>
       </c>
       <c r="G108" s="27">
-        <v>6423</v>
+        <v>9374</v>
       </c>
     </row>
     <row r="109" spans="1:7">
-      <c r="A109" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B109" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C109" s="35" t="s">
-        <v>26</v>
+      <c r="A109" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B109" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C109" s="31" t="s">
+        <v>21</v>
       </c>
       <c r="D109"/>
       <c r="E109" s="27" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F109" s="27">
-        <v>6424</v>
+        <v>9378</v>
       </c>
       <c r="G109" s="27">
-        <v>7797</v>
+        <v>9646</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -8054,13 +8201,13 @@
       </c>
       <c r="D110"/>
       <c r="E110" s="27" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="F110" s="27">
-        <v>7798</v>
+        <v>1</v>
       </c>
       <c r="G110" s="27">
-        <v>9498</v>
+        <v>9867</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -8075,491 +8222,491 @@
       </c>
       <c r="D111"/>
       <c r="E111" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F111" s="27">
+        <v>1</v>
+      </c>
+      <c r="G111" s="27">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B112" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C112" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D112"/>
+      <c r="E112" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F112" s="27">
+        <v>328</v>
+      </c>
+      <c r="G112" s="27">
+        <v>9501</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B113" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C113" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D113"/>
+      <c r="E113" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F113" s="27">
+        <v>328</v>
+      </c>
+      <c r="G113" s="27">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B114" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C114" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D114"/>
+      <c r="E114" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="F114" s="27">
+        <v>328</v>
+      </c>
+      <c r="G114" s="27">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B115" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C115" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D115"/>
+      <c r="E115" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F115" s="27">
+        <v>565</v>
+      </c>
+      <c r="G115" s="27">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B116" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C116" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D116"/>
+      <c r="E116" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F116" s="27">
+        <v>1138</v>
+      </c>
+      <c r="G116" s="27">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B117" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C117" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D117"/>
+      <c r="E117" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F117" s="27">
+        <v>2200</v>
+      </c>
+      <c r="G117" s="27">
+        <v>2910</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B118" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C118" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D118"/>
+      <c r="E118" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F118" s="27">
+        <v>2911</v>
+      </c>
+      <c r="G118" s="27">
+        <v>9498</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B119" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C119" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D119"/>
+      <c r="E119" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="F119" s="27">
+        <v>2911</v>
+      </c>
+      <c r="G119" s="27">
+        <v>3630</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B120" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C120" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D120"/>
+      <c r="E120" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F120" s="27">
+        <v>3631</v>
+      </c>
+      <c r="G120" s="27">
+        <v>5514</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B121" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C121" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D121"/>
+      <c r="E121" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="F121" s="27">
+        <v>5515</v>
+      </c>
+      <c r="G121" s="27">
+        <v>5637</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B122" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C122" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D122"/>
+      <c r="E122" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="F122" s="27">
+        <v>5638</v>
+      </c>
+      <c r="G122" s="27">
+        <v>6423</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B123" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C123" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D123"/>
+      <c r="E123" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F123" s="27">
+        <v>6424</v>
+      </c>
+      <c r="G123" s="27">
+        <v>7797</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B124" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C124" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D124"/>
+      <c r="E124" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F124" s="27">
+        <v>7798</v>
+      </c>
+      <c r="G124" s="27">
+        <v>9498</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B125" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C125" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D125"/>
+      <c r="E125" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F111" s="27">
+      <c r="F125" s="27">
         <v>9502</v>
       </c>
-      <c r="G111" s="27">
+      <c r="G125" s="27">
         <v>9867</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
-      <c r="A112" t="s">
+    <row r="126" spans="1:7">
+      <c r="A126" t="s">
         <v>54</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B126" t="s">
         <v>63</v>
       </c>
-      <c r="C112" s="16" t="s">
+      <c r="C126" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D112" s="22" t="s">
+      <c r="D126" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="E112" s="27" t="s">
+      <c r="E126" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="F112" s="27">
+      <c r="F126" s="27">
         <v>1</v>
       </c>
-      <c r="G112" s="27">
+      <c r="G126" s="27">
         <v>19199</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
-      <c r="A113" t="s">
+    <row r="127" spans="1:7">
+      <c r="A127" t="s">
         <v>54</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B127" t="s">
         <v>63</v>
       </c>
-      <c r="C113" s="16" t="s">
+      <c r="C127" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D113" s="22" t="s">
+      <c r="D127" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="E113" s="27" t="s">
+      <c r="E127" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F113" s="27">
+      <c r="F127" s="27">
         <v>1</v>
       </c>
-      <c r="G113" s="27">
+      <c r="G127" s="27">
         <v>350</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
-      <c r="A114" t="s">
+    <row r="128" spans="1:7">
+      <c r="A128" t="s">
         <v>54</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B128" t="s">
         <v>63</v>
       </c>
-      <c r="C114" s="16" t="s">
+      <c r="C128" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D114" s="22" t="s">
+      <c r="D128" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="E114" s="27" t="s">
+      <c r="E128" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="F114" s="27">
+      <c r="F128" s="27">
         <v>351</v>
       </c>
-      <c r="G114" s="27">
+      <c r="G128" s="27">
         <v>18068</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
-      <c r="A115" t="s">
+    <row r="129" spans="1:7">
+      <c r="A129" t="s">
         <v>54</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B129" t="s">
         <v>63</v>
       </c>
-      <c r="C115" s="16" t="s">
+      <c r="C129" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D115" s="22" t="s">
+      <c r="D129" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="E115" s="27" t="s">
+      <c r="E129" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F115" s="27">
+      <c r="F129" s="27">
         <v>18069</v>
       </c>
-      <c r="G115" s="27">
+      <c r="G129" s="27">
         <v>19199</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
-      <c r="A116" s="32" t="s">
+    <row r="130" spans="1:7">
+      <c r="A130" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B116" s="32" t="s">
+      <c r="B130" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C116" s="33" t="s">
+      <c r="C130" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D116" s="27" t="s">
+      <c r="D130" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="E116" s="27" t="s">
+      <c r="E130" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="F116" s="27">
+      <c r="F130" s="27">
         <v>1</v>
       </c>
-      <c r="G116" s="27">
+      <c r="G130" s="27">
         <v>18554</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
-      <c r="A117" s="34" t="s">
+    <row r="131" spans="1:7">
+      <c r="A131" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="B117" s="32" t="s">
+      <c r="B131" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C117" s="33" t="s">
+      <c r="C131" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D117" s="27" t="s">
+      <c r="D131" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="E117" s="27" t="s">
+      <c r="E131" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F117" s="27">
+      <c r="F131" s="27">
         <v>1</v>
       </c>
-      <c r="G117" s="27">
+      <c r="G131" s="27">
         <v>199</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
-      <c r="A118" s="34" t="s">
+    <row r="132" spans="1:7">
+      <c r="A132" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="B118" s="32" t="s">
+      <c r="B132" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C118" s="33" t="s">
+      <c r="C132" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D118" s="27" t="s">
+      <c r="D132" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="E118" s="27" t="s">
+      <c r="E132" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="F118" s="27">
+      <c r="F132" s="27">
         <v>200</v>
       </c>
-      <c r="G118" s="27">
+      <c r="G132" s="27">
         <v>17905</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
-      <c r="A119" s="34" t="s">
+    <row r="133" spans="1:7">
+      <c r="A133" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="B119" s="32" t="s">
+      <c r="B133" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C119" s="33" t="s">
+      <c r="C133" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D119" s="27" t="s">
+      <c r="D133" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="E119" s="27" t="s">
+      <c r="E133" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F119" s="27">
+      <c r="F133" s="27">
         <v>17906</v>
       </c>
-      <c r="G119" s="27">
+      <c r="G133" s="27">
         <v>18554</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7">
-      <c r="A120" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B120" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C120" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D120" s="27"/>
-      <c r="E120" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F120" s="27">
-        <v>1</v>
-      </c>
-      <c r="G120" s="27">
-        <v>12573</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7">
-      <c r="A121" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B121" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C121" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D121" s="27"/>
-      <c r="E121" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F121" s="27">
-        <v>1</v>
-      </c>
-      <c r="G121" s="27">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7">
-      <c r="A122" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B122" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C122" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D122" s="27"/>
-      <c r="E122" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F122" s="27">
-        <v>386</v>
-      </c>
-      <c r="G122" s="27">
-        <v>12352</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7">
-      <c r="A123" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B123" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C123" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D123" s="27"/>
-      <c r="E123" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F123" s="27">
-        <v>386</v>
-      </c>
-      <c r="G123" s="27">
-        <v>3583</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7">
-      <c r="A124" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B124" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C124" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D124" s="27"/>
-      <c r="E124" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="F124" s="27">
-        <v>386</v>
-      </c>
-      <c r="G124" s="27">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7">
-      <c r="A125" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B125" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C125" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D125" s="27"/>
-      <c r="E125" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F125" s="27">
-        <v>890</v>
-      </c>
-      <c r="G125" s="27">
-        <v>1195</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7">
-      <c r="A126" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B126" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C126" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D126" s="27"/>
-      <c r="E126" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="F126" s="27">
-        <v>1196</v>
-      </c>
-      <c r="G126" s="27">
-        <v>1876</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7">
-      <c r="A127" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B127" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C127" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D127" s="27"/>
-      <c r="E127" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="F127" s="27">
-        <v>1877</v>
-      </c>
-      <c r="G127" s="27">
-        <v>2461</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7">
-      <c r="A128" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B128" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C128" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D128" s="27"/>
-      <c r="E128" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="F128" s="27">
-        <v>2462</v>
-      </c>
-      <c r="G128" s="27">
-        <v>3583</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7">
-      <c r="A129" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B129" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C129" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D129" s="27"/>
-      <c r="E129" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="F129" s="27">
-        <v>3584</v>
-      </c>
-      <c r="G129" s="27">
-        <v>3793</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7">
-      <c r="A130" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B130" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C130" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D130" s="27"/>
-      <c r="E130" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F130" s="27">
-        <v>3794</v>
-      </c>
-      <c r="G130" s="27">
-        <v>7471</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7">
-      <c r="A131" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B131" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C131" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D131" s="27"/>
-      <c r="E131" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="F131" s="27">
-        <v>7472</v>
-      </c>
-      <c r="G131" s="27">
-        <v>7663</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7">
-      <c r="A132" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B132" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C132" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D132" s="27"/>
-      <c r="E132" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="F132" s="27">
-        <v>7664</v>
-      </c>
-      <c r="G132" s="27">
-        <v>8704</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7">
-      <c r="A133" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B133" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C133" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D133" s="27"/>
-      <c r="E133" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F133" s="27">
-        <v>8705</v>
-      </c>
-      <c r="G133" s="27">
-        <v>10192</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -8574,13 +8721,13 @@
       </c>
       <c r="D134" s="27"/>
       <c r="E134" s="27" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="F134" s="27">
-        <v>10193</v>
+        <v>1</v>
       </c>
       <c r="G134" s="27">
-        <v>12349</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -8595,310 +8742,310 @@
       </c>
       <c r="D135" s="27"/>
       <c r="E135" s="27" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F135" s="27">
-        <v>12360</v>
+        <v>1</v>
       </c>
       <c r="G135" s="27">
-        <v>12573</v>
+        <v>385</v>
       </c>
     </row>
     <row r="136" spans="1:7">
-      <c r="A136" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B136" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C136" s="27" t="s">
-        <v>57</v>
+      <c r="A136" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B136" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C136" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D136" s="27"/>
       <c r="E136" s="27" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="F136" s="27">
-        <v>1</v>
+        <v>386</v>
       </c>
       <c r="G136" s="27">
-        <v>10053</v>
+        <v>12352</v>
       </c>
     </row>
     <row r="137" spans="1:7">
-      <c r="A137" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B137" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C137" s="27" t="s">
-        <v>57</v>
+      <c r="A137" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B137" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C137" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D137" s="27"/>
       <c r="E137" s="27" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="F137" s="27">
-        <v>1</v>
+        <v>386</v>
       </c>
       <c r="G137" s="27">
-        <v>10053</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="138" spans="1:7">
-      <c r="A138" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B138" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C138" s="27" t="s">
-        <v>57</v>
+      <c r="A138" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B138" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C138" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D138" s="27"/>
       <c r="E138" s="27" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="F138" s="27">
-        <v>1</v>
+        <v>386</v>
       </c>
       <c r="G138" s="27">
-        <v>2358</v>
+        <v>889</v>
       </c>
     </row>
     <row r="139" spans="1:7">
-      <c r="A139" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B139" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C139" s="27" t="s">
-        <v>57</v>
+      <c r="A139" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B139" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C139" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D139" s="27"/>
       <c r="E139" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F139" s="27">
-        <v>1</v>
+        <v>890</v>
       </c>
       <c r="G139" s="27">
-        <v>345</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="140" spans="1:7">
-      <c r="A140" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B140" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C140" s="27" t="s">
-        <v>57</v>
+      <c r="A140" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B140" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C140" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D140" s="27"/>
       <c r="E140" s="27" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="F140" s="27">
-        <v>346</v>
+        <v>1196</v>
       </c>
       <c r="G140" s="27">
-        <v>852</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="141" spans="1:7">
-      <c r="A141" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B141" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C141" s="27" t="s">
-        <v>57</v>
+      <c r="A141" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B141" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C141" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D141" s="27"/>
       <c r="E141" s="27" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="F141" s="27">
-        <v>655</v>
+        <v>1877</v>
       </c>
       <c r="G141" s="27">
-        <v>852</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="142" spans="1:7">
-      <c r="A142" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B142" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C142" s="27" t="s">
-        <v>57</v>
+      <c r="A142" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B142" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C142" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D142" s="27"/>
       <c r="E142" s="27" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F142" s="27">
-        <v>853</v>
+        <v>2462</v>
       </c>
       <c r="G142" s="27">
-        <v>2358</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="143" spans="1:7">
-      <c r="A143" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B143" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C143" s="27" t="s">
-        <v>57</v>
+      <c r="A143" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B143" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C143" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D143" s="27"/>
       <c r="E143" s="27" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="F143" s="27">
-        <v>2359</v>
+        <v>3584</v>
       </c>
       <c r="G143" s="27">
-        <v>10050</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="144" spans="1:7">
-      <c r="A144" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B144" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C144" s="27" t="s">
-        <v>57</v>
+      <c r="A144" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B144" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C144" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D144" s="27"/>
       <c r="E144" s="27" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F144" s="27">
-        <v>2359</v>
+        <v>3794</v>
       </c>
       <c r="G144" s="27">
-        <v>3390</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8">
-      <c r="A145" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B145" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C145" s="27" t="s">
-        <v>57</v>
+        <v>7471</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B145" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C145" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D145" s="27"/>
       <c r="E145" s="27" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="F145" s="27">
-        <v>3391</v>
+        <v>7472</v>
       </c>
       <c r="G145" s="27">
-        <v>3978</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8">
-      <c r="A146" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B146" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C146" s="27" t="s">
-        <v>57</v>
+        <v>7663</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B146" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C146" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D146" s="27"/>
       <c r="E146" s="27" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="F146" s="27">
-        <v>3979</v>
+        <v>7664</v>
       </c>
       <c r="G146" s="27">
-        <v>4431</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8">
-      <c r="A147" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B147" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C147" s="27" t="s">
-        <v>57</v>
+        <v>8704</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B147" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C147" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D147" s="27"/>
       <c r="E147" s="27" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F147" s="27">
-        <v>4432</v>
+        <v>8705</v>
       </c>
       <c r="G147" s="27">
-        <v>6303</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8">
-      <c r="A148" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B148" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C148" s="27" t="s">
-        <v>57</v>
+        <v>10192</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B148" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C148" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D148" s="27"/>
       <c r="E148" s="27" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="F148" s="27">
-        <v>6304</v>
+        <v>10193</v>
       </c>
       <c r="G148" s="27">
-        <v>6687</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8">
-      <c r="A149" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B149" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C149" s="27" t="s">
-        <v>57</v>
+        <v>12349</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B149" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C149" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D149" s="27"/>
       <c r="E149" s="27" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F149" s="27">
-        <v>6688</v>
+        <v>12360</v>
       </c>
       <c r="G149" s="27">
-        <v>6762</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8">
+        <v>12573</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
       <c r="A150" s="27" t="s">
         <v>52</v>
       </c>
@@ -8910,16 +9057,16 @@
       </c>
       <c r="D150" s="27"/>
       <c r="E150" s="27" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F150" s="27">
-        <v>6763</v>
+        <v>1</v>
       </c>
       <c r="G150" s="27">
-        <v>7557</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8">
+        <v>10053</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
       <c r="A151" s="27" t="s">
         <v>52</v>
       </c>
@@ -8931,182 +9078,451 @@
       </c>
       <c r="D151" s="27"/>
       <c r="E151" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F151" s="27">
+        <v>1</v>
+      </c>
+      <c r="G151" s="27">
+        <v>10053</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B152" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C152" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D152" s="27"/>
+      <c r="E152" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F152" s="27">
+        <v>1</v>
+      </c>
+      <c r="G152" s="27">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B153" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C153" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D153" s="27"/>
+      <c r="E153" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F153" s="27">
+        <v>1</v>
+      </c>
+      <c r="G153" s="27">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B154" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C154" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D154" s="27"/>
+      <c r="E154" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F154" s="27">
+        <v>346</v>
+      </c>
+      <c r="G154" s="27">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B155" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C155" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D155" s="27"/>
+      <c r="E155" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F155" s="27">
+        <v>655</v>
+      </c>
+      <c r="G155" s="27">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="A156" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B156" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C156" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D156" s="27"/>
+      <c r="E156" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F156" s="27">
+        <v>853</v>
+      </c>
+      <c r="G156" s="27">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B157" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C157" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D157" s="27"/>
+      <c r="E157" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F157" s="27">
+        <v>2359</v>
+      </c>
+      <c r="G157" s="27">
+        <v>10050</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B158" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C158" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D158" s="27"/>
+      <c r="E158" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F158" s="27">
+        <v>2359</v>
+      </c>
+      <c r="G158" s="27">
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B159" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C159" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D159" s="27"/>
+      <c r="E159" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="F159" s="27">
+        <v>3391</v>
+      </c>
+      <c r="G159" s="27">
+        <v>3978</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B160" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C160" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D160" s="27"/>
+      <c r="E160" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="F160" s="27">
+        <v>3979</v>
+      </c>
+      <c r="G160" s="27">
+        <v>4431</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8">
+      <c r="A161" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B161" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C161" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D161" s="27"/>
+      <c r="E161" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F161" s="27">
+        <v>4432</v>
+      </c>
+      <c r="G161" s="27">
+        <v>6303</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8">
+      <c r="A162" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B162" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C162" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D162" s="27"/>
+      <c r="E162" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F162" s="27">
+        <v>6304</v>
+      </c>
+      <c r="G162" s="27">
+        <v>6687</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8">
+      <c r="A163" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B163" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C163" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D163" s="27"/>
+      <c r="E163" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F163" s="27">
+        <v>6688</v>
+      </c>
+      <c r="G163" s="27">
+        <v>6762</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8">
+      <c r="A164" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B164" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C164" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D164" s="27"/>
+      <c r="E164" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F164" s="27">
+        <v>6763</v>
+      </c>
+      <c r="G164" s="27">
+        <v>7557</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8">
+      <c r="A165" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B165" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C165" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D165" s="27"/>
+      <c r="E165" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="F151" s="27">
+      <c r="F165" s="27">
         <v>7558</v>
       </c>
-      <c r="G151" s="27">
+      <c r="G165" s="27">
         <v>10050</v>
       </c>
-      <c r="H151" s="25"/>
-    </row>
-    <row r="152" spans="1:8">
-      <c r="A152" s="27" t="s">
+      <c r="H165" s="25"/>
+    </row>
+    <row r="166" spans="1:8">
+      <c r="A166" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B152" s="27" t="s">
+      <c r="B166" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C152" s="27" t="s">
+      <c r="C166" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D152" s="27" t="s">
+      <c r="D166" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="E152" s="27" t="s">
+      <c r="E166" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="F152" s="27">
+      <c r="F166" s="27">
         <v>105</v>
       </c>
-      <c r="G152" s="27">
+      <c r="G166" s="27">
         <v>2849</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
-      <c r="A153" t="s">
+    <row r="167" spans="1:8">
+      <c r="A167" t="s">
         <v>113</v>
       </c>
-      <c r="B153" s="27" t="s">
+      <c r="B167" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="C153" s="27" t="s">
+      <c r="C167" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D153" s="27" t="s">
+      <c r="D167" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="E153" s="27" t="s">
+      <c r="E167" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F153" s="27">
+      <c r="F167" s="27">
         <v>117</v>
       </c>
-      <c r="G153" s="27">
+      <c r="G167" s="27">
         <v>2543</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
-      <c r="A154" s="27" t="s">
+    <row r="168" spans="1:8">
+      <c r="A168" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B154" s="27" t="s">
+      <c r="B168" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C154" s="27" t="s">
+      <c r="C168" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D154" s="27" t="s">
+      <c r="D168" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="E154" s="27" t="s">
+      <c r="E168" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="F154" s="27">
+      <c r="F168" s="27">
+        <v>105</v>
+      </c>
+      <c r="G168" s="27">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8">
+      <c r="A169" t="s">
+        <v>113</v>
+      </c>
+      <c r="B169" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C169" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D169" t="s">
+        <v>112</v>
+      </c>
+      <c r="E169" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F169" s="27">
+        <v>117</v>
+      </c>
+      <c r="G169" s="27">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8">
+      <c r="A170" t="s">
+        <v>108</v>
+      </c>
+      <c r="B170" t="s">
+        <v>65</v>
+      </c>
+      <c r="C170" t="s">
+        <v>109</v>
+      </c>
+      <c r="D170" t="s">
+        <v>112</v>
+      </c>
+      <c r="E170" t="s">
+        <v>83</v>
+      </c>
+      <c r="F170">
         <v>1</v>
       </c>
-      <c r="G154" s="27">
+      <c r="G170">
         <v>3114</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
-      <c r="A155" t="s">
+    <row r="171" spans="1:8">
+      <c r="A171" t="s">
         <v>113</v>
       </c>
-      <c r="B155" s="27" t="s">
+      <c r="B171" t="s">
         <v>114</v>
       </c>
-      <c r="C155" s="27" t="s">
+      <c r="C171" t="s">
         <v>109</v>
       </c>
-      <c r="D155" s="27" t="s">
+      <c r="D171" t="s">
         <v>112</v>
       </c>
-      <c r="E155" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F155" s="27">
+      <c r="E171" t="s">
+        <v>83</v>
+      </c>
+      <c r="F171">
         <v>1</v>
       </c>
-      <c r="G155" s="27">
+      <c r="G171">
         <v>2824</v>
       </c>
-    </row>
-    <row r="193" spans="2:4">
-      <c r="B193" s="1"/>
-      <c r="C193" s="5"/>
-      <c r="D193" s="5"/>
-    </row>
-    <row r="194" spans="2:4">
-      <c r="B194" s="1"/>
-      <c r="C194" s="5"/>
-      <c r="D194" s="5"/>
-    </row>
-    <row r="195" spans="2:4">
-      <c r="B195" s="1"/>
-      <c r="C195" s="5"/>
-      <c r="D195" s="5"/>
-    </row>
-    <row r="196" spans="2:4">
-      <c r="B196" s="1"/>
-      <c r="C196" s="5"/>
-      <c r="D196" s="5"/>
-    </row>
-    <row r="197" spans="2:4">
-      <c r="B197" s="1"/>
-      <c r="C197" s="5"/>
-      <c r="D197" s="5"/>
-    </row>
-    <row r="198" spans="2:4">
-      <c r="B198" s="1"/>
-      <c r="C198" s="5"/>
-      <c r="D198" s="5"/>
-    </row>
-    <row r="199" spans="2:4">
-      <c r="B199" s="1"/>
-      <c r="C199" s="5"/>
-      <c r="D199" s="5"/>
-    </row>
-    <row r="200" spans="2:4">
-      <c r="B200" s="1"/>
-      <c r="C200" s="5"/>
-      <c r="D200" s="5"/>
-    </row>
-    <row r="201" spans="2:4">
-      <c r="B201" s="1"/>
-      <c r="C201" s="5"/>
-      <c r="D201" s="5"/>
-    </row>
-    <row r="202" spans="2:4">
-      <c r="B202" s="1"/>
-      <c r="C202" s="5"/>
-      <c r="D202" s="5"/>
-    </row>
-    <row r="203" spans="2:4">
-      <c r="B203" s="1"/>
-      <c r="C203" s="5"/>
-      <c r="D203" s="5"/>
-    </row>
-    <row r="204" spans="2:4">
-      <c r="B204" s="1"/>
-      <c r="C204" s="5"/>
-      <c r="D204" s="5"/>
-    </row>
-    <row r="205" spans="2:4">
-      <c r="B205" s="1"/>
-      <c r="C205" s="5"/>
-      <c r="D205" s="5"/>
-    </row>
-    <row r="206" spans="2:4">
-      <c r="B206" s="1"/>
-      <c r="C206" s="5"/>
-      <c r="D206" s="5"/>
     </row>
     <row r="207" spans="2:4">
       <c r="B207" s="1"/>
       <c r="C207" s="5"/>
-      <c r="D207" s="5"/>
     </row>
     <row r="208" spans="2:4">
       <c r="B208" s="1"/>
@@ -9155,6 +9571,8 @@
     </row>
     <row r="217" spans="2:4">
       <c r="B217" s="1"/>
+      <c r="C217" s="5"/>
+      <c r="D217" s="5"/>
     </row>
     <row r="218" spans="2:4">
       <c r="B218" s="1"/>
@@ -9191,178 +9609,249 @@
       <c r="C224" s="5"/>
       <c r="D224" s="5"/>
     </row>
-    <row r="907" spans="5:5">
-      <c r="E907" s="1"/>
-    </row>
-    <row r="1043" spans="2:2">
-      <c r="B1043" s="1"/>
-    </row>
-    <row r="1044" spans="2:2">
-      <c r="B1044" s="1"/>
-    </row>
-    <row r="1169" spans="2:2">
-      <c r="B1169" s="1"/>
-    </row>
-    <row r="1170" spans="2:2">
-      <c r="B1170" s="1"/>
-    </row>
-    <row r="1171" spans="2:2">
-      <c r="B1171" s="1"/>
-    </row>
-    <row r="1172" spans="2:2">
-      <c r="B1172" s="1"/>
-    </row>
-    <row r="1173" spans="2:2">
-      <c r="B1173" s="1"/>
-    </row>
-    <row r="1174" spans="2:2">
-      <c r="B1174" s="1"/>
-    </row>
-    <row r="1219" spans="2:6">
-      <c r="E1219" s="1"/>
-      <c r="F1219" s="1"/>
-    </row>
-    <row r="1220" spans="2:6">
-      <c r="E1220" s="1"/>
-      <c r="F1220" s="1"/>
-    </row>
-    <row r="1221" spans="2:6">
-      <c r="E1221" s="1"/>
-      <c r="F1221" s="1"/>
-    </row>
-    <row r="1223" spans="2:6">
-      <c r="B1223" s="1"/>
-    </row>
-    <row r="1224" spans="2:6">
-      <c r="B1224" s="1"/>
-    </row>
-    <row r="1225" spans="2:6">
-      <c r="B1225" s="1"/>
-    </row>
-    <row r="1226" spans="2:6">
-      <c r="B1226" s="1"/>
-    </row>
-    <row r="1227" spans="2:6">
-      <c r="B1227" s="1"/>
-    </row>
-    <row r="1246" spans="2:2">
-      <c r="B1246" s="1"/>
-    </row>
-    <row r="1247" spans="2:2">
-      <c r="B1247" s="1"/>
-    </row>
-    <row r="1248" spans="2:2">
-      <c r="B1248" s="1"/>
-    </row>
-    <row r="1249" spans="2:2">
-      <c r="B1249" s="1"/>
-    </row>
-    <row r="1250" spans="2:2">
-      <c r="B1250" s="1"/>
-    </row>
-    <row r="1251" spans="2:2">
-      <c r="B1251" s="1"/>
-    </row>
-    <row r="1252" spans="2:2">
-      <c r="B1252" s="1"/>
-    </row>
-    <row r="1254" spans="2:2">
-      <c r="B1254" s="1"/>
-    </row>
-    <row r="1255" spans="2:2">
-      <c r="B1255" s="1"/>
-    </row>
-    <row r="1256" spans="2:2">
-      <c r="B1256" s="1"/>
-    </row>
-    <row r="1257" spans="2:2">
-      <c r="B1257" s="1"/>
-    </row>
-    <row r="1258" spans="2:2">
-      <c r="B1258" s="1"/>
-    </row>
-    <row r="1259" spans="2:2">
-      <c r="B1259" s="1"/>
-    </row>
-    <row r="1311" spans="2:2">
-      <c r="B1311" s="1"/>
-    </row>
-    <row r="1312" spans="2:2">
-      <c r="B1312" s="1"/>
-    </row>
-    <row r="1313" spans="2:2">
-      <c r="B1313" s="1"/>
-    </row>
-    <row r="1314" spans="2:2">
-      <c r="B1314" s="1"/>
-    </row>
-    <row r="1316" spans="2:2">
-      <c r="B1316" s="1"/>
-    </row>
-    <row r="1317" spans="2:2">
-      <c r="B1317" s="1"/>
-    </row>
-    <row r="1318" spans="2:2">
-      <c r="B1318" s="1"/>
-    </row>
-    <row r="1319" spans="2:2">
-      <c r="B1319" s="1"/>
-    </row>
-    <row r="1354" spans="2:2">
-      <c r="B1354" s="1"/>
-    </row>
-    <row r="1355" spans="2:2">
-      <c r="B1355" s="1"/>
-    </row>
-    <row r="1356" spans="2:2">
-      <c r="B1356" s="1"/>
-    </row>
-    <row r="1357" spans="2:2">
-      <c r="B1357" s="1"/>
-    </row>
-    <row r="1358" spans="2:2">
-      <c r="B1358" s="1"/>
-    </row>
-    <row r="1359" spans="2:2">
-      <c r="B1359" s="1"/>
-    </row>
-    <row r="1401" spans="3:6">
-      <c r="E1401" s="1"/>
-      <c r="F1401" s="1"/>
-    </row>
-    <row r="1402" spans="3:6">
-      <c r="C1402" s="6"/>
-      <c r="D1402" s="6"/>
-      <c r="E1402" s="1"/>
-      <c r="F1402" s="1"/>
-    </row>
-    <row r="1403" spans="3:6">
-      <c r="C1403" s="6"/>
-      <c r="D1403" s="6"/>
-      <c r="E1403" s="1"/>
-      <c r="F1403" s="1"/>
-    </row>
-    <row r="1404" spans="3:6">
-      <c r="C1404" s="6"/>
-      <c r="D1404" s="6"/>
-      <c r="E1404" s="1"/>
-      <c r="F1404" s="1"/>
-    </row>
-    <row r="1405" spans="3:6">
-      <c r="E1405" s="1"/>
-      <c r="F1405" s="1"/>
-    </row>
-    <row r="1468" spans="2:2">
-      <c r="B1468" s="1"/>
-    </row>
-    <row r="1469" spans="2:2">
-      <c r="B1469" s="1"/>
-    </row>
-    <row r="1470" spans="2:2">
-      <c r="B1470" s="1"/>
-    </row>
-    <row r="1471" spans="2:2">
-      <c r="B1471" s="1"/>
+    <row r="225" spans="2:4">
+      <c r="B225" s="1"/>
+      <c r="C225" s="5"/>
+      <c r="D225" s="5"/>
+    </row>
+    <row r="226" spans="2:4">
+      <c r="B226" s="1"/>
+      <c r="C226" s="5"/>
+      <c r="D226" s="5"/>
+    </row>
+    <row r="227" spans="2:4">
+      <c r="B227" s="1"/>
+      <c r="C227" s="5"/>
+      <c r="D227" s="5"/>
+    </row>
+    <row r="228" spans="2:4">
+      <c r="B228" s="1"/>
+      <c r="C228" s="5"/>
+      <c r="D228" s="5"/>
+    </row>
+    <row r="229" spans="2:4">
+      <c r="B229" s="1"/>
+      <c r="C229" s="5"/>
+      <c r="D229" s="5"/>
+    </row>
+    <row r="230" spans="2:4">
+      <c r="B230" s="1"/>
+      <c r="C230" s="5"/>
+      <c r="D230" s="5"/>
+    </row>
+    <row r="231" spans="2:4">
+      <c r="B231" s="1"/>
+      <c r="D231" s="5"/>
+    </row>
+    <row r="232" spans="2:4">
+      <c r="B232" s="1"/>
+      <c r="C232" s="5"/>
+    </row>
+    <row r="233" spans="2:4">
+      <c r="B233" s="1"/>
+      <c r="C233" s="5"/>
+      <c r="D233" s="5"/>
+    </row>
+    <row r="234" spans="2:4">
+      <c r="B234" s="1"/>
+      <c r="C234" s="5"/>
+      <c r="D234" s="5"/>
+    </row>
+    <row r="235" spans="2:4">
+      <c r="B235" s="1"/>
+      <c r="C235" s="5"/>
+      <c r="D235" s="5"/>
+    </row>
+    <row r="236" spans="2:4">
+      <c r="B236" s="1"/>
+      <c r="C236" s="5"/>
+      <c r="D236" s="5"/>
+    </row>
+    <row r="237" spans="2:4">
+      <c r="B237" s="1"/>
+      <c r="C237" s="5"/>
+      <c r="D237" s="5"/>
+    </row>
+    <row r="238" spans="2:4">
+      <c r="B238" s="1"/>
+      <c r="C238" s="5"/>
+      <c r="D238" s="5"/>
+    </row>
+    <row r="239" spans="2:4">
+      <c r="D239" s="5"/>
+    </row>
+    <row r="921" spans="5:5">
+      <c r="E921" s="1"/>
+    </row>
+    <row r="1057" spans="2:2">
+      <c r="B1057" s="1"/>
+    </row>
+    <row r="1058" spans="2:2">
+      <c r="B1058" s="1"/>
+    </row>
+    <row r="1183" spans="2:2">
+      <c r="B1183" s="1"/>
+    </row>
+    <row r="1184" spans="2:2">
+      <c r="B1184" s="1"/>
+    </row>
+    <row r="1185" spans="2:2">
+      <c r="B1185" s="1"/>
+    </row>
+    <row r="1186" spans="2:2">
+      <c r="B1186" s="1"/>
+    </row>
+    <row r="1187" spans="2:2">
+      <c r="B1187" s="1"/>
+    </row>
+    <row r="1188" spans="2:2">
+      <c r="B1188" s="1"/>
+    </row>
+    <row r="1233" spans="2:6">
+      <c r="E1233" s="1"/>
+      <c r="F1233" s="1"/>
+    </row>
+    <row r="1234" spans="2:6">
+      <c r="E1234" s="1"/>
+      <c r="F1234" s="1"/>
+    </row>
+    <row r="1235" spans="2:6">
+      <c r="E1235" s="1"/>
+      <c r="F1235" s="1"/>
+    </row>
+    <row r="1237" spans="2:6">
+      <c r="B1237" s="1"/>
+    </row>
+    <row r="1238" spans="2:6">
+      <c r="B1238" s="1"/>
+    </row>
+    <row r="1239" spans="2:6">
+      <c r="B1239" s="1"/>
+    </row>
+    <row r="1240" spans="2:6">
+      <c r="B1240" s="1"/>
+    </row>
+    <row r="1241" spans="2:6">
+      <c r="B1241" s="1"/>
+    </row>
+    <row r="1260" spans="2:2">
+      <c r="B1260" s="1"/>
+    </row>
+    <row r="1261" spans="2:2">
+      <c r="B1261" s="1"/>
+    </row>
+    <row r="1262" spans="2:2">
+      <c r="B1262" s="1"/>
+    </row>
+    <row r="1263" spans="2:2">
+      <c r="B1263" s="1"/>
+    </row>
+    <row r="1264" spans="2:2">
+      <c r="B1264" s="1"/>
+    </row>
+    <row r="1265" spans="2:2">
+      <c r="B1265" s="1"/>
+    </row>
+    <row r="1266" spans="2:2">
+      <c r="B1266" s="1"/>
+    </row>
+    <row r="1268" spans="2:2">
+      <c r="B1268" s="1"/>
+    </row>
+    <row r="1269" spans="2:2">
+      <c r="B1269" s="1"/>
+    </row>
+    <row r="1270" spans="2:2">
+      <c r="B1270" s="1"/>
+    </row>
+    <row r="1271" spans="2:2">
+      <c r="B1271" s="1"/>
+    </row>
+    <row r="1272" spans="2:2">
+      <c r="B1272" s="1"/>
+    </row>
+    <row r="1273" spans="2:2">
+      <c r="B1273" s="1"/>
+    </row>
+    <row r="1325" spans="2:2">
+      <c r="B1325" s="1"/>
+    </row>
+    <row r="1326" spans="2:2">
+      <c r="B1326" s="1"/>
+    </row>
+    <row r="1327" spans="2:2">
+      <c r="B1327" s="1"/>
+    </row>
+    <row r="1328" spans="2:2">
+      <c r="B1328" s="1"/>
+    </row>
+    <row r="1330" spans="2:2">
+      <c r="B1330" s="1"/>
+    </row>
+    <row r="1331" spans="2:2">
+      <c r="B1331" s="1"/>
+    </row>
+    <row r="1332" spans="2:2">
+      <c r="B1332" s="1"/>
+    </row>
+    <row r="1333" spans="2:2">
+      <c r="B1333" s="1"/>
+    </row>
+    <row r="1368" spans="2:2">
+      <c r="B1368" s="1"/>
+    </row>
+    <row r="1369" spans="2:2">
+      <c r="B1369" s="1"/>
+    </row>
+    <row r="1370" spans="2:2">
+      <c r="B1370" s="1"/>
+    </row>
+    <row r="1371" spans="2:2">
+      <c r="B1371" s="1"/>
+    </row>
+    <row r="1372" spans="2:2">
+      <c r="B1372" s="1"/>
+    </row>
+    <row r="1373" spans="2:2">
+      <c r="B1373" s="1"/>
+    </row>
+    <row r="1415" spans="3:6">
+      <c r="E1415" s="1"/>
+      <c r="F1415" s="1"/>
+    </row>
+    <row r="1416" spans="3:6">
+      <c r="C1416" s="6"/>
+      <c r="E1416" s="1"/>
+      <c r="F1416" s="1"/>
+    </row>
+    <row r="1417" spans="3:6">
+      <c r="C1417" s="6"/>
+      <c r="D1417" s="6"/>
+      <c r="E1417" s="1"/>
+      <c r="F1417" s="1"/>
+    </row>
+    <row r="1418" spans="3:6">
+      <c r="C1418" s="6"/>
+      <c r="D1418" s="6"/>
+      <c r="E1418" s="1"/>
+      <c r="F1418" s="1"/>
+    </row>
+    <row r="1419" spans="3:6">
+      <c r="D1419" s="6"/>
+      <c r="E1419" s="1"/>
+      <c r="F1419" s="1"/>
+    </row>
+    <row r="1482" spans="2:2">
+      <c r="B1482" s="1"/>
+    </row>
+    <row r="1483" spans="2:2">
+      <c r="B1483" s="1"/>
+    </row>
+    <row r="1484" spans="2:2">
+      <c r="B1484" s="1"/>
+    </row>
+    <row r="1485" spans="2:2">
+      <c r="B1485" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:G1456">

</xml_diff>

<commit_message>
Added missing features and FASTA export
</commit_message>
<xml_diff>
--- a/tabular/virus/flavi-reference_feature_locations.xlsx
+++ b/tabular/virus/flavi-reference_feature_locations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1660" yWindow="0" windowWidth="25560" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="115">
   <si>
     <t>featureName</t>
   </si>
@@ -588,9 +588,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2403">
+  <cellStyleXfs count="2429">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3065,7 +3091,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2403">
+  <cellStyles count="2429">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -4268,6 +4294,19 @@
     <cellStyle name="Followed Hyperlink" xfId="2398" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2400" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2428" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -5468,6 +5507,19 @@
     <cellStyle name="Hyperlink" xfId="2397" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2399" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2427" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5805,10 +5857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1499"/>
+  <dimension ref="A1:H1502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6698,25 +6750,25 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="36" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F39" s="26">
-        <v>16</v>
-      </c>
-      <c r="G39" s="26">
-        <v>10320</v>
+        <v>60</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="28">
+        <v>1</v>
+      </c>
+      <c r="G39" s="28">
+        <v>10735</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -6733,13 +6785,13 @@
         <v>39</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="F40" s="28">
         <v>1</v>
       </c>
       <c r="G40" s="28">
-        <v>10735</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -6756,13 +6808,13 @@
         <v>39</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" s="28">
-        <v>1</v>
-      </c>
-      <c r="G41" s="28">
-        <v>94</v>
+        <v>70</v>
+      </c>
+      <c r="F41" s="27">
+        <v>95</v>
+      </c>
+      <c r="G41" s="27">
+        <v>10273</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -6778,14 +6830,14 @@
       <c r="D42" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="27" t="s">
-        <v>70</v>
+      <c r="E42" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="F42" s="27">
         <v>95</v>
       </c>
       <c r="G42" s="27">
-        <v>10273</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -6801,14 +6853,14 @@
       <c r="D43" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E43" s="29" t="s">
-        <v>105</v>
+      <c r="E43" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="F43" s="27">
         <v>95</v>
       </c>
       <c r="G43" s="27">
-        <v>2419</v>
+        <v>436</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -6825,13 +6877,13 @@
         <v>39</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="F44" s="27">
-        <v>95</v>
+        <v>437</v>
       </c>
       <c r="G44" s="27">
-        <v>436</v>
+        <v>934</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -6848,13 +6900,13 @@
         <v>39</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F45" s="27">
-        <v>437</v>
+        <v>935</v>
       </c>
       <c r="G45" s="27">
-        <v>934</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -6871,13 +6923,13 @@
         <v>39</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="F46" s="27">
-        <v>935</v>
+        <v>2420</v>
       </c>
       <c r="G46" s="27">
-        <v>2419</v>
+        <v>10270</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -6894,13 +6946,13 @@
         <v>39</v>
       </c>
       <c r="E47" s="27" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
       <c r="F47" s="27">
         <v>2420</v>
       </c>
       <c r="G47" s="27">
-        <v>10270</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -6917,13 +6969,13 @@
         <v>39</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="F48" s="27">
-        <v>2420</v>
+        <v>3476</v>
       </c>
       <c r="G48" s="27">
-        <v>3475</v>
+        <v>4129</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -6940,13 +6992,13 @@
         <v>39</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F49" s="27">
-        <v>3476</v>
+        <v>4130</v>
       </c>
       <c r="G49" s="27">
-        <v>4129</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -6963,13 +7015,13 @@
         <v>39</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="F50" s="27">
-        <v>4130</v>
+        <v>4520</v>
       </c>
       <c r="G50" s="27">
-        <v>4519</v>
+        <v>6376</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -6986,13 +7038,13 @@
         <v>39</v>
       </c>
       <c r="E51" s="27" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="F51" s="27">
-        <v>4520</v>
+        <v>6377</v>
       </c>
       <c r="G51" s="27">
-        <v>6376</v>
+        <v>6757</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -7009,13 +7061,13 @@
         <v>39</v>
       </c>
       <c r="E52" s="27" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="F52" s="27">
-        <v>6377</v>
+        <v>6758</v>
       </c>
       <c r="G52" s="27">
-        <v>6757</v>
+        <v>6826</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -7032,13 +7084,13 @@
         <v>39</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="F53" s="27">
-        <v>6758</v>
+        <v>6827</v>
       </c>
       <c r="G53" s="27">
-        <v>6826</v>
+        <v>7573</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -7055,7 +7107,7 @@
         <v>39</v>
       </c>
       <c r="E54" s="27" t="s">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="F54" s="27">
         <v>7574</v>
@@ -8597,13 +8649,13 @@
         <v>107</v>
       </c>
       <c r="E121" s="27" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F121" s="27">
         <v>6258</v>
       </c>
       <c r="G121" s="27">
-        <v>7601</v>
+        <v>9374</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -8620,13 +8672,13 @@
         <v>107</v>
       </c>
       <c r="E122" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F122" s="27">
-        <v>7602</v>
+        <v>6258</v>
       </c>
       <c r="G122" s="27">
-        <v>9374</v>
+        <v>7601</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -8643,34 +8695,36 @@
         <v>107</v>
       </c>
       <c r="E123" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F123" s="27">
+        <v>7602</v>
+      </c>
+      <c r="G123" s="27">
+        <v>9374</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B124" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C124" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D124" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E124" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F123" s="27">
+      <c r="F124" s="27">
         <v>9378</v>
       </c>
-      <c r="G123" s="27">
+      <c r="G124" s="27">
         <v>9646</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7">
-      <c r="A124" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B124" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C124" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D124"/>
-      <c r="E124" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F124" s="27">
-        <v>1</v>
-      </c>
-      <c r="G124" s="27">
-        <v>9867</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -8685,13 +8739,13 @@
       </c>
       <c r="D125"/>
       <c r="E125" s="27" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F125" s="27">
         <v>1</v>
       </c>
       <c r="G125" s="27">
-        <v>327</v>
+        <v>9867</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -8706,13 +8760,13 @@
       </c>
       <c r="D126"/>
       <c r="E126" s="27" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F126" s="27">
-        <v>328</v>
+        <v>1</v>
       </c>
       <c r="G126" s="27">
-        <v>9501</v>
+        <v>327</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -8727,13 +8781,13 @@
       </c>
       <c r="D127"/>
       <c r="E127" s="27" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="F127" s="27">
         <v>328</v>
       </c>
       <c r="G127" s="27">
-        <v>2199</v>
+        <v>9501</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -8748,13 +8802,13 @@
       </c>
       <c r="D128"/>
       <c r="E128" s="27" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="F128" s="27">
         <v>328</v>
       </c>
       <c r="G128" s="27">
-        <v>564</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -8769,13 +8823,13 @@
       </c>
       <c r="D129"/>
       <c r="E129" s="27" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="F129" s="27">
-        <v>565</v>
+        <v>328</v>
       </c>
       <c r="G129" s="27">
-        <v>1137</v>
+        <v>564</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -8790,13 +8844,13 @@
       </c>
       <c r="D130"/>
       <c r="E130" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F130" s="27">
-        <v>1138</v>
+        <v>565</v>
       </c>
       <c r="G130" s="27">
-        <v>2199</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -8811,13 +8865,13 @@
       </c>
       <c r="D131"/>
       <c r="E131" s="27" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="F131" s="27">
-        <v>2200</v>
+        <v>1138</v>
       </c>
       <c r="G131" s="27">
-        <v>2910</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -8832,13 +8886,13 @@
       </c>
       <c r="D132"/>
       <c r="E132" s="27" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="F132" s="27">
-        <v>2911</v>
+        <v>2200</v>
       </c>
       <c r="G132" s="27">
-        <v>9498</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -8853,13 +8907,13 @@
       </c>
       <c r="D133"/>
       <c r="E133" s="27" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F133" s="27">
         <v>2911</v>
       </c>
       <c r="G133" s="27">
-        <v>3630</v>
+        <v>9498</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -8874,13 +8928,13 @@
       </c>
       <c r="D134"/>
       <c r="E134" s="27" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="F134" s="27">
-        <v>3631</v>
+        <v>2911</v>
       </c>
       <c r="G134" s="27">
-        <v>5514</v>
+        <v>3630</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -8895,13 +8949,13 @@
       </c>
       <c r="D135"/>
       <c r="E135" s="27" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="F135" s="27">
-        <v>5515</v>
+        <v>3631</v>
       </c>
       <c r="G135" s="27">
-        <v>5637</v>
+        <v>5514</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -8916,13 +8970,13 @@
       </c>
       <c r="D136"/>
       <c r="E136" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F136" s="27">
-        <v>5638</v>
+        <v>5515</v>
       </c>
       <c r="G136" s="27">
-        <v>6423</v>
+        <v>5637</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -8937,13 +8991,13 @@
       </c>
       <c r="D137"/>
       <c r="E137" s="27" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="F137" s="27">
-        <v>6424</v>
+        <v>5638</v>
       </c>
       <c r="G137" s="27">
-        <v>7797</v>
+        <v>6423</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -8958,10 +9012,10 @@
       </c>
       <c r="D138"/>
       <c r="E138" s="27" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F138" s="27">
-        <v>7798</v>
+        <v>6424</v>
       </c>
       <c r="G138" s="27">
         <v>9498</v>
@@ -8979,59 +9033,55 @@
       </c>
       <c r="D139"/>
       <c r="E139" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F139" s="27">
+        <v>6424</v>
+      </c>
+      <c r="G139" s="27">
+        <v>7797</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B140" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C140" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D140"/>
+      <c r="E140" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F140" s="27">
+        <v>7798</v>
+      </c>
+      <c r="G140" s="27">
+        <v>9498</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B141" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C141" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D141"/>
+      <c r="E141" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F139" s="27">
+      <c r="F141" s="27">
         <v>9502</v>
       </c>
-      <c r="G139" s="27">
+      <c r="G141" s="27">
         <v>9867</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7">
-      <c r="A140" t="s">
-        <v>54</v>
-      </c>
-      <c r="B140" t="s">
-        <v>63</v>
-      </c>
-      <c r="C140" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D140" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="E140" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F140" s="27">
-        <v>1</v>
-      </c>
-      <c r="G140" s="27">
-        <v>19199</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7">
-      <c r="A141" t="s">
-        <v>54</v>
-      </c>
-      <c r="B141" t="s">
-        <v>63</v>
-      </c>
-      <c r="C141" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D141" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="E141" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F141" s="27">
-        <v>1</v>
-      </c>
-      <c r="G141" s="27">
-        <v>350</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -9048,13 +9098,13 @@
         <v>110</v>
       </c>
       <c r="E142" s="27" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F142" s="27">
-        <v>351</v>
+        <v>1</v>
       </c>
       <c r="G142" s="27">
-        <v>18068</v>
+        <v>19199</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -9071,63 +9121,63 @@
         <v>110</v>
       </c>
       <c r="E143" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F143" s="27">
+        <v>1</v>
+      </c>
+      <c r="G143" s="27">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" t="s">
+        <v>54</v>
+      </c>
+      <c r="B144" t="s">
+        <v>63</v>
+      </c>
+      <c r="C144" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D144" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="E144" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F144" s="27">
+        <v>351</v>
+      </c>
+      <c r="G144" s="27">
+        <v>18068</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" t="s">
+        <v>54</v>
+      </c>
+      <c r="B145" t="s">
+        <v>63</v>
+      </c>
+      <c r="C145" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D145" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="E145" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F143" s="27">
+      <c r="F145" s="27">
         <v>18069</v>
       </c>
-      <c r="G143" s="27">
+      <c r="G145" s="27">
         <v>19199</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
-      <c r="A144" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B144" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C144" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="D144" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E144" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F144" s="27">
-        <v>1</v>
-      </c>
-      <c r="G144" s="27">
-        <v>18554</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7">
-      <c r="A145" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B145" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C145" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="D145" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E145" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F145" s="27">
-        <v>1</v>
-      </c>
-      <c r="G145" s="27">
-        <v>199</v>
-      </c>
-    </row>
     <row r="146" spans="1:7">
-      <c r="A146" s="34" t="s">
+      <c r="A146" s="32" t="s">
         <v>84</v>
       </c>
       <c r="B146" s="32" t="s">
@@ -9140,13 +9190,13 @@
         <v>111</v>
       </c>
       <c r="E146" s="27" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F146" s="27">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="G146" s="27">
-        <v>17905</v>
+        <v>18554</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -9163,55 +9213,59 @@
         <v>111</v>
       </c>
       <c r="E147" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F147" s="27">
+        <v>1</v>
+      </c>
+      <c r="G147" s="27">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B148" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C148" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D148" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E148" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F148" s="27">
+        <v>200</v>
+      </c>
+      <c r="G148" s="27">
+        <v>17905</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B149" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C149" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D149" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E149" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F147" s="27">
+      <c r="F149" s="27">
         <v>17906</v>
       </c>
-      <c r="G147" s="27">
+      <c r="G149" s="27">
         <v>18554</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7">
-      <c r="A148" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B148" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C148" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D148" s="27"/>
-      <c r="E148" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F148" s="27">
-        <v>1</v>
-      </c>
-      <c r="G148" s="27">
-        <v>12573</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7">
-      <c r="A149" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B149" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C149" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D149" s="27"/>
-      <c r="E149" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F149" s="27">
-        <v>1</v>
-      </c>
-      <c r="G149" s="27">
-        <v>385</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -9226,13 +9280,13 @@
       </c>
       <c r="D150" s="27"/>
       <c r="E150" s="27" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F150" s="27">
-        <v>386</v>
+        <v>1</v>
       </c>
       <c r="G150" s="27">
-        <v>12352</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -9247,13 +9301,13 @@
       </c>
       <c r="D151" s="27"/>
       <c r="E151" s="27" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="F151" s="27">
-        <v>386</v>
+        <v>1</v>
       </c>
       <c r="G151" s="27">
-        <v>3583</v>
+        <v>385</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -9268,13 +9322,13 @@
       </c>
       <c r="D152" s="27"/>
       <c r="E152" s="27" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F152" s="27">
         <v>386</v>
       </c>
       <c r="G152" s="27">
-        <v>889</v>
+        <v>12352</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -9289,13 +9343,13 @@
       </c>
       <c r="D153" s="27"/>
       <c r="E153" s="27" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="F153" s="27">
-        <v>890</v>
+        <v>386</v>
       </c>
       <c r="G153" s="27">
-        <v>1195</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -9310,13 +9364,13 @@
       </c>
       <c r="D154" s="27"/>
       <c r="E154" s="27" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="F154" s="27">
-        <v>1196</v>
+        <v>386</v>
       </c>
       <c r="G154" s="27">
-        <v>1876</v>
+        <v>889</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -9331,13 +9385,13 @@
       </c>
       <c r="D155" s="27"/>
       <c r="E155" s="27" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F155" s="27">
-        <v>1877</v>
+        <v>890</v>
       </c>
       <c r="G155" s="27">
-        <v>2461</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -9352,13 +9406,13 @@
       </c>
       <c r="D156" s="27"/>
       <c r="E156" s="27" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="F156" s="27">
-        <v>2462</v>
+        <v>1196</v>
       </c>
       <c r="G156" s="27">
-        <v>3583</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -9373,13 +9427,13 @@
       </c>
       <c r="D157" s="27"/>
       <c r="E157" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F157" s="27">
-        <v>3584</v>
+        <v>1877</v>
       </c>
       <c r="G157" s="27">
-        <v>3793</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -9394,13 +9448,13 @@
       </c>
       <c r="D158" s="27"/>
       <c r="E158" s="27" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="F158" s="27">
-        <v>3794</v>
+        <v>2462</v>
       </c>
       <c r="G158" s="27">
-        <v>7471</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -9415,13 +9469,13 @@
       </c>
       <c r="D159" s="27"/>
       <c r="E159" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F159" s="27">
-        <v>7472</v>
+        <v>3584</v>
       </c>
       <c r="G159" s="27">
-        <v>7663</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -9436,13 +9490,13 @@
       </c>
       <c r="D160" s="27"/>
       <c r="E160" s="27" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="F160" s="27">
-        <v>7664</v>
+        <v>3794</v>
       </c>
       <c r="G160" s="27">
-        <v>8704</v>
+        <v>7471</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -9457,13 +9511,13 @@
       </c>
       <c r="D161" s="27"/>
       <c r="E161" s="27" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="F161" s="27">
-        <v>8705</v>
+        <v>7472</v>
       </c>
       <c r="G161" s="27">
-        <v>10192</v>
+        <v>7663</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -9478,13 +9532,13 @@
       </c>
       <c r="D162" s="27"/>
       <c r="E162" s="27" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="F162" s="27">
-        <v>10193</v>
+        <v>7664</v>
       </c>
       <c r="G162" s="27">
-        <v>12349</v>
+        <v>8704</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -9499,76 +9553,76 @@
       </c>
       <c r="D163" s="27"/>
       <c r="E163" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F163" s="27">
-        <v>12360</v>
+        <v>8705</v>
       </c>
       <c r="G163" s="27">
-        <v>12573</v>
+        <v>12349</v>
       </c>
     </row>
     <row r="164" spans="1:7">
-      <c r="A164" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B164" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C164" s="27" t="s">
-        <v>57</v>
+      <c r="A164" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B164" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C164" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D164" s="27"/>
       <c r="E164" s="27" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="F164" s="27">
-        <v>1</v>
+        <v>8705</v>
       </c>
       <c r="G164" s="27">
-        <v>10053</v>
+        <v>10192</v>
       </c>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B165" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C165" s="27" t="s">
-        <v>57</v>
+      <c r="A165" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B165" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C165" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D165" s="27"/>
       <c r="E165" s="27" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="F165" s="27">
-        <v>1</v>
+        <v>10193</v>
       </c>
       <c r="G165" s="27">
-        <v>10053</v>
+        <v>12349</v>
       </c>
     </row>
     <row r="166" spans="1:7">
-      <c r="A166" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B166" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C166" s="27" t="s">
-        <v>57</v>
+      <c r="A166" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B166" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C166" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D166" s="27"/>
       <c r="E166" s="27" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="F166" s="27">
-        <v>1</v>
+        <v>12360</v>
       </c>
       <c r="G166" s="27">
-        <v>2358</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -9583,13 +9637,13 @@
       </c>
       <c r="D167" s="27"/>
       <c r="E167" s="27" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F167" s="27">
         <v>1</v>
       </c>
       <c r="G167" s="27">
-        <v>345</v>
+        <v>10053</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -9604,13 +9658,13 @@
       </c>
       <c r="D168" s="27"/>
       <c r="E168" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F168" s="27">
-        <v>346</v>
+        <v>1</v>
       </c>
       <c r="G168" s="27">
-        <v>852</v>
+        <v>10053</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -9625,13 +9679,13 @@
       </c>
       <c r="D169" s="27"/>
       <c r="E169" s="27" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="F169" s="27">
-        <v>655</v>
+        <v>1</v>
       </c>
       <c r="G169" s="27">
-        <v>852</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -9646,13 +9700,13 @@
       </c>
       <c r="D170" s="27"/>
       <c r="E170" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F170" s="27">
-        <v>853</v>
+        <v>1</v>
       </c>
       <c r="G170" s="27">
-        <v>2358</v>
+        <v>345</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -9667,13 +9721,13 @@
       </c>
       <c r="D171" s="27"/>
       <c r="E171" s="27" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="F171" s="27">
-        <v>2359</v>
+        <v>346</v>
       </c>
       <c r="G171" s="27">
-        <v>10050</v>
+        <v>852</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -9688,13 +9742,13 @@
       </c>
       <c r="D172" s="27"/>
       <c r="E172" s="27" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="F172" s="27">
-        <v>2359</v>
+        <v>655</v>
       </c>
       <c r="G172" s="27">
-        <v>3390</v>
+        <v>852</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -9709,13 +9763,13 @@
       </c>
       <c r="D173" s="27"/>
       <c r="E173" s="27" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F173" s="27">
-        <v>3391</v>
+        <v>853</v>
       </c>
       <c r="G173" s="27">
-        <v>3978</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -9730,13 +9784,13 @@
       </c>
       <c r="D174" s="27"/>
       <c r="E174" s="27" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F174" s="27">
-        <v>3979</v>
+        <v>2359</v>
       </c>
       <c r="G174" s="27">
-        <v>4431</v>
+        <v>10050</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -9751,13 +9805,13 @@
       </c>
       <c r="D175" s="27"/>
       <c r="E175" s="27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F175" s="27">
-        <v>4432</v>
+        <v>2359</v>
       </c>
       <c r="G175" s="27">
-        <v>6303</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -9772,13 +9826,13 @@
       </c>
       <c r="D176" s="27"/>
       <c r="E176" s="27" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F176" s="27">
-        <v>6304</v>
+        <v>3391</v>
       </c>
       <c r="G176" s="27">
-        <v>6687</v>
+        <v>3978</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -9793,13 +9847,13 @@
       </c>
       <c r="D177" s="27"/>
       <c r="E177" s="27" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="F177" s="27">
-        <v>6688</v>
+        <v>3979</v>
       </c>
       <c r="G177" s="27">
-        <v>6762</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -9814,13 +9868,13 @@
       </c>
       <c r="D178" s="27"/>
       <c r="E178" s="27" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="F178" s="27">
-        <v>6763</v>
+        <v>4432</v>
       </c>
       <c r="G178" s="27">
-        <v>7557</v>
+        <v>6303</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -9835,172 +9889,220 @@
       </c>
       <c r="D179" s="27"/>
       <c r="E179" s="27" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="F179" s="27">
-        <v>7558</v>
+        <v>6304</v>
       </c>
       <c r="G179" s="27">
-        <v>10050</v>
-      </c>
-      <c r="H179" s="25"/>
+        <v>6687</v>
+      </c>
     </row>
     <row r="180" spans="1:8">
       <c r="A180" s="27" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
       <c r="B180" s="27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C180" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D180" s="27" t="s">
-        <v>112</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D180" s="27"/>
       <c r="E180" s="27" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F180" s="27">
-        <v>105</v>
+        <v>6688</v>
       </c>
       <c r="G180" s="27">
-        <v>2849</v>
+        <v>6762</v>
       </c>
     </row>
     <row r="181" spans="1:8">
-      <c r="A181" t="s">
-        <v>113</v>
+      <c r="A181" s="27" t="s">
+        <v>52</v>
       </c>
       <c r="B181" s="27" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
       <c r="C181" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D181" s="27" t="s">
-        <v>112</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D181" s="27"/>
       <c r="E181" s="27" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="F181" s="27">
-        <v>117</v>
+        <v>6763</v>
       </c>
       <c r="G181" s="27">
-        <v>2543</v>
+        <v>7557</v>
       </c>
     </row>
     <row r="182" spans="1:8">
       <c r="A182" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B182" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C182" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D182" s="27"/>
+      <c r="E182" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F182" s="27">
+        <v>7558</v>
+      </c>
+      <c r="G182" s="27">
+        <v>10050</v>
+      </c>
+      <c r="H182" s="25"/>
+    </row>
+    <row r="183" spans="1:8">
+      <c r="A183" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B182" s="27" t="s">
+      <c r="B183" s="27" t="s">
         <v>65</v>
-      </c>
-      <c r="C182" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D182" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E182" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F182" s="27">
-        <v>105</v>
-      </c>
-      <c r="G182" s="27">
-        <v>2849</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8">
-      <c r="A183" t="s">
-        <v>113</v>
-      </c>
-      <c r="B183" s="27" t="s">
-        <v>114</v>
       </c>
       <c r="C183" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="27" t="s">
         <v>112</v>
       </c>
       <c r="E183" s="27" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F183" s="27">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G183" s="27">
-        <v>2543</v>
+        <v>2849</v>
       </c>
     </row>
     <row r="184" spans="1:8">
       <c r="A184" t="s">
+        <v>113</v>
+      </c>
+      <c r="B184" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C184" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D184" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E184" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F184" s="27">
+        <v>117</v>
+      </c>
+      <c r="G184" s="27">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8">
+      <c r="A185" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B185" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C185" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D185" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E185" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F185" s="27">
+        <v>105</v>
+      </c>
+      <c r="G185" s="27">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8">
+      <c r="A186" t="s">
+        <v>113</v>
+      </c>
+      <c r="B186" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C186" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D186" t="s">
+        <v>112</v>
+      </c>
+      <c r="E186" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F186" s="27">
+        <v>117</v>
+      </c>
+      <c r="G186" s="27">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8">
+      <c r="A187" t="s">
+        <v>108</v>
+      </c>
+      <c r="B187" t="s">
+        <v>65</v>
+      </c>
+      <c r="C187" t="s">
+        <v>109</v>
+      </c>
+      <c r="D187" t="s">
+        <v>112</v>
+      </c>
+      <c r="E187" t="s">
         <v>83</v>
       </c>
-      <c r="F184">
+      <c r="F187">
         <v>1</v>
       </c>
-      <c r="G184">
+      <c r="G187">
         <v>3114</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
-      <c r="A185" t="s">
+    <row r="188" spans="1:8">
+      <c r="A188" t="s">
         <v>113</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B188" t="s">
         <v>114</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C188" t="s">
         <v>109</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D188" t="s">
         <v>112</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E188" t="s">
         <v>83</v>
       </c>
-      <c r="F185">
+      <c r="F188">
         <v>1</v>
       </c>
-      <c r="G185">
+      <c r="G188">
         <v>2824</v>
       </c>
     </row>
-    <row r="221" spans="2:4">
-      <c r="B221" s="1"/>
-      <c r="C221" s="5"/>
-    </row>
-    <row r="222" spans="2:4">
-      <c r="B222" s="1"/>
-      <c r="C222" s="5"/>
-      <c r="D222" s="5"/>
-    </row>
-    <row r="223" spans="2:4">
-      <c r="B223" s="1"/>
-      <c r="C223" s="5"/>
-      <c r="D223" s="5"/>
-    </row>
-    <row r="224" spans="2:4">
+    <row r="224" spans="2:3">
       <c r="B224" s="1"/>
       <c r="C224" s="5"/>
-      <c r="D224" s="5"/>
     </row>
     <row r="225" spans="2:4">
       <c r="B225" s="1"/>
@@ -10104,11 +10206,13 @@
     </row>
     <row r="245" spans="2:4">
       <c r="B245" s="1"/>
+      <c r="C245" s="5"/>
       <c r="D245" s="5"/>
     </row>
     <row r="246" spans="2:4">
       <c r="B246" s="1"/>
       <c r="C246" s="5"/>
+      <c r="D246" s="5"/>
     </row>
     <row r="247" spans="2:4">
       <c r="B247" s="1"/>
@@ -10117,13 +10221,11 @@
     </row>
     <row r="248" spans="2:4">
       <c r="B248" s="1"/>
-      <c r="C248" s="5"/>
       <c r="D248" s="5"/>
     </row>
     <row r="249" spans="2:4">
       <c r="B249" s="1"/>
       <c r="C249" s="5"/>
-      <c r="D249" s="5"/>
     </row>
     <row r="250" spans="2:4">
       <c r="B250" s="1"/>
@@ -10141,25 +10243,31 @@
       <c r="D252" s="5"/>
     </row>
     <row r="253" spans="2:4">
+      <c r="B253" s="1"/>
+      <c r="C253" s="5"/>
       <c r="D253" s="5"/>
     </row>
-    <row r="935" spans="5:5">
-      <c r="E935" s="1"/>
-    </row>
-    <row r="1071" spans="2:2">
-      <c r="B1071" s="1"/>
-    </row>
-    <row r="1072" spans="2:2">
-      <c r="B1072" s="1"/>
-    </row>
-    <row r="1197" spans="2:2">
-      <c r="B1197" s="1"/>
-    </row>
-    <row r="1198" spans="2:2">
-      <c r="B1198" s="1"/>
-    </row>
-    <row r="1199" spans="2:2">
-      <c r="B1199" s="1"/>
+    <row r="254" spans="2:4">
+      <c r="B254" s="1"/>
+      <c r="C254" s="5"/>
+      <c r="D254" s="5"/>
+    </row>
+    <row r="255" spans="2:4">
+      <c r="B255" s="1"/>
+      <c r="C255" s="5"/>
+      <c r="D255" s="5"/>
+    </row>
+    <row r="256" spans="2:4">
+      <c r="D256" s="5"/>
+    </row>
+    <row r="938" spans="5:5">
+      <c r="E938" s="1"/>
+    </row>
+    <row r="1074" spans="2:2">
+      <c r="B1074" s="1"/>
+    </row>
+    <row r="1075" spans="2:2">
+      <c r="B1075" s="1"/>
     </row>
     <row r="1200" spans="2:2">
       <c r="B1200" s="1"/>
@@ -10170,26 +10278,26 @@
     <row r="1202" spans="2:2">
       <c r="B1202" s="1"/>
     </row>
-    <row r="1247" spans="5:6">
-      <c r="E1247" s="1"/>
-      <c r="F1247" s="1"/>
-    </row>
-    <row r="1248" spans="5:6">
-      <c r="E1248" s="1"/>
-      <c r="F1248" s="1"/>
-    </row>
-    <row r="1249" spans="2:6">
-      <c r="E1249" s="1"/>
-      <c r="F1249" s="1"/>
+    <row r="1203" spans="2:2">
+      <c r="B1203" s="1"/>
+    </row>
+    <row r="1204" spans="2:2">
+      <c r="B1204" s="1"/>
+    </row>
+    <row r="1205" spans="2:2">
+      <c r="B1205" s="1"/>
+    </row>
+    <row r="1250" spans="2:6">
+      <c r="E1250" s="1"/>
+      <c r="F1250" s="1"/>
     </row>
     <row r="1251" spans="2:6">
-      <c r="B1251" s="1"/>
+      <c r="E1251" s="1"/>
+      <c r="F1251" s="1"/>
     </row>
     <row r="1252" spans="2:6">
-      <c r="B1252" s="1"/>
-    </row>
-    <row r="1253" spans="2:6">
-      <c r="B1253" s="1"/>
+      <c r="E1252" s="1"/>
+      <c r="F1252" s="1"/>
     </row>
     <row r="1254" spans="2:6">
       <c r="B1254" s="1"/>
@@ -10197,14 +10305,14 @@
     <row r="1255" spans="2:6">
       <c r="B1255" s="1"/>
     </row>
-    <row r="1274" spans="2:2">
-      <c r="B1274" s="1"/>
-    </row>
-    <row r="1275" spans="2:2">
-      <c r="B1275" s="1"/>
-    </row>
-    <row r="1276" spans="2:2">
-      <c r="B1276" s="1"/>
+    <row r="1256" spans="2:6">
+      <c r="B1256" s="1"/>
+    </row>
+    <row r="1257" spans="2:6">
+      <c r="B1257" s="1"/>
+    </row>
+    <row r="1258" spans="2:6">
+      <c r="B1258" s="1"/>
     </row>
     <row r="1277" spans="2:2">
       <c r="B1277" s="1"/>
@@ -10218,15 +10326,15 @@
     <row r="1280" spans="2:2">
       <c r="B1280" s="1"/>
     </row>
+    <row r="1281" spans="2:2">
+      <c r="B1281" s="1"/>
+    </row>
     <row r="1282" spans="2:2">
       <c r="B1282" s="1"/>
     </row>
     <row r="1283" spans="2:2">
       <c r="B1283" s="1"/>
     </row>
-    <row r="1284" spans="2:2">
-      <c r="B1284" s="1"/>
-    </row>
     <row r="1285" spans="2:2">
       <c r="B1285" s="1"/>
     </row>
@@ -10236,38 +10344,38 @@
     <row r="1287" spans="2:2">
       <c r="B1287" s="1"/>
     </row>
-    <row r="1339" spans="2:2">
-      <c r="B1339" s="1"/>
-    </row>
-    <row r="1340" spans="2:2">
-      <c r="B1340" s="1"/>
-    </row>
-    <row r="1341" spans="2:2">
-      <c r="B1341" s="1"/>
+    <row r="1288" spans="2:2">
+      <c r="B1288" s="1"/>
+    </row>
+    <row r="1289" spans="2:2">
+      <c r="B1289" s="1"/>
+    </row>
+    <row r="1290" spans="2:2">
+      <c r="B1290" s="1"/>
     </row>
     <row r="1342" spans="2:2">
       <c r="B1342" s="1"/>
     </row>
+    <row r="1343" spans="2:2">
+      <c r="B1343" s="1"/>
+    </row>
     <row r="1344" spans="2:2">
       <c r="B1344" s="1"/>
     </row>
     <row r="1345" spans="2:2">
       <c r="B1345" s="1"/>
     </row>
-    <row r="1346" spans="2:2">
-      <c r="B1346" s="1"/>
-    </row>
     <row r="1347" spans="2:2">
       <c r="B1347" s="1"/>
     </row>
-    <row r="1382" spans="2:2">
-      <c r="B1382" s="1"/>
-    </row>
-    <row r="1383" spans="2:2">
-      <c r="B1383" s="1"/>
-    </row>
-    <row r="1384" spans="2:2">
-      <c r="B1384" s="1"/>
+    <row r="1348" spans="2:2">
+      <c r="B1348" s="1"/>
+    </row>
+    <row r="1349" spans="2:2">
+      <c r="B1349" s="1"/>
+    </row>
+    <row r="1350" spans="2:2">
+      <c r="B1350" s="1"/>
     </row>
     <row r="1385" spans="2:2">
       <c r="B1385" s="1"/>
@@ -10278,43 +10386,52 @@
     <row r="1387" spans="2:2">
       <c r="B1387" s="1"/>
     </row>
-    <row r="1429" spans="3:6">
-      <c r="E1429" s="1"/>
-      <c r="F1429" s="1"/>
-    </row>
-    <row r="1430" spans="3:6">
-      <c r="C1430" s="6"/>
-      <c r="E1430" s="1"/>
-      <c r="F1430" s="1"/>
-    </row>
-    <row r="1431" spans="3:6">
-      <c r="C1431" s="6"/>
-      <c r="D1431" s="6"/>
-      <c r="E1431" s="1"/>
-      <c r="F1431" s="1"/>
+    <row r="1388" spans="2:2">
+      <c r="B1388" s="1"/>
+    </row>
+    <row r="1389" spans="2:2">
+      <c r="B1389" s="1"/>
+    </row>
+    <row r="1390" spans="2:2">
+      <c r="B1390" s="1"/>
     </row>
     <row r="1432" spans="3:6">
-      <c r="C1432" s="6"/>
-      <c r="D1432" s="6"/>
       <c r="E1432" s="1"/>
       <c r="F1432" s="1"/>
     </row>
     <row r="1433" spans="3:6">
-      <c r="D1433" s="6"/>
+      <c r="C1433" s="6"/>
       <c r="E1433" s="1"/>
       <c r="F1433" s="1"/>
     </row>
-    <row r="1496" spans="2:2">
-      <c r="B1496" s="1"/>
-    </row>
-    <row r="1497" spans="2:2">
-      <c r="B1497" s="1"/>
-    </row>
-    <row r="1498" spans="2:2">
-      <c r="B1498" s="1"/>
+    <row r="1434" spans="3:6">
+      <c r="C1434" s="6"/>
+      <c r="D1434" s="6"/>
+      <c r="E1434" s="1"/>
+      <c r="F1434" s="1"/>
+    </row>
+    <row r="1435" spans="3:6">
+      <c r="C1435" s="6"/>
+      <c r="D1435" s="6"/>
+      <c r="E1435" s="1"/>
+      <c r="F1435" s="1"/>
+    </row>
+    <row r="1436" spans="3:6">
+      <c r="D1436" s="6"/>
+      <c r="E1436" s="1"/>
+      <c r="F1436" s="1"/>
     </row>
     <row r="1499" spans="2:2">
       <c r="B1499" s="1"/>
+    </row>
+    <row r="1500" spans="2:2">
+      <c r="B1500" s="1"/>
+    </row>
+    <row r="1501" spans="2:2">
+      <c r="B1501" s="1"/>
+    </row>
+    <row r="1502" spans="2:2">
+      <c r="B1502" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:G1456">

</xml_diff>

<commit_message>
Updated feature location data and logic
</commit_message>
<xml_diff>
--- a/tabular/virus/flavi-reference_feature_locations.xlsx
+++ b/tabular/virus/flavi-reference_feature_locations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="118">
   <si>
     <t>featureName</t>
   </si>
@@ -368,6 +368,15 @@
   </si>
   <si>
     <t>REF_JMTV_SEG3</t>
+  </si>
+  <si>
+    <t>Crustacean</t>
+  </si>
+  <si>
+    <t>MK473878</t>
+  </si>
+  <si>
+    <t>REF_ccCFV</t>
   </si>
 </sst>
 </file>
@@ -439,7 +448,7 @@
       <name val="Courier"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,6 +587,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -588,7 +603,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2439">
+  <cellStyleXfs count="2457">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3028,8 +3043,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3100,8 +3133,12 @@
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2439">
+  <cellStyles count="2457">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -4322,6 +4359,15 @@
     <cellStyle name="Followed Hyperlink" xfId="2434" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2436" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2456" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -5540,6 +5586,15 @@
     <cellStyle name="Hyperlink" xfId="2433" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2435" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2455" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5877,10 +5932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1502"/>
+  <dimension ref="A1:H1503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F21" sqref="A1:G188"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E95" sqref="A1:G189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7966,26 +8021,26 @@
       </c>
     </row>
     <row r="91" spans="1:8">
-      <c r="A91" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B91" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C91" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D91" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E91" s="27" t="s">
+      <c r="A91" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="B91" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="C91" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="E91" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F91" s="27">
+      <c r="F91" s="1">
         <v>1</v>
       </c>
-      <c r="G91" s="27">
-        <v>10839</v>
+      <c r="G91" s="1">
+        <v>11434</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -8002,13 +8057,13 @@
         <v>43</v>
       </c>
       <c r="E92" s="27" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F92" s="27">
         <v>1</v>
       </c>
       <c r="G92" s="27">
-        <v>111</v>
+        <v>10839</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -8025,13 +8080,13 @@
         <v>43</v>
       </c>
       <c r="E93" s="27" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F93" s="27">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="G93" s="27">
-        <v>10359</v>
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -8048,13 +8103,13 @@
         <v>43</v>
       </c>
       <c r="E94" s="27" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="F94" s="27">
         <v>112</v>
       </c>
       <c r="G94" s="27">
-        <v>2436</v>
+        <v>10359</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -8071,13 +8126,13 @@
         <v>43</v>
       </c>
       <c r="E95" s="27" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="F95" s="27">
         <v>112</v>
       </c>
       <c r="G95" s="27">
-        <v>441</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -8094,13 +8149,13 @@
         <v>43</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="F96" s="27">
-        <v>442</v>
+        <v>112</v>
       </c>
       <c r="G96" s="27">
-        <v>945</v>
+        <v>441</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -8117,13 +8172,13 @@
         <v>43</v>
       </c>
       <c r="E97" s="27" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="F97" s="27">
-        <v>946</v>
+        <v>442</v>
       </c>
       <c r="G97" s="27">
-        <v>2436</v>
+        <v>945</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -8140,13 +8195,13 @@
         <v>43</v>
       </c>
       <c r="E98" s="27" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="F98" s="27">
-        <v>2437</v>
+        <v>946</v>
       </c>
       <c r="G98" s="27">
-        <v>10356</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -8163,13 +8218,13 @@
         <v>43</v>
       </c>
       <c r="E99" s="27" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
       <c r="F99" s="27">
         <v>2437</v>
       </c>
       <c r="G99" s="27">
-        <v>3495</v>
+        <v>10356</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -8186,13 +8241,13 @@
         <v>43</v>
       </c>
       <c r="E100" s="27" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="F100" s="27">
-        <v>3496</v>
+        <v>2437</v>
       </c>
       <c r="G100" s="27">
-        <v>4185</v>
+        <v>3495</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -8209,13 +8264,13 @@
         <v>43</v>
       </c>
       <c r="E101" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F101" s="27">
-        <v>4186</v>
+        <v>3496</v>
       </c>
       <c r="G101" s="27">
-        <v>4578</v>
+        <v>4185</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -8232,13 +8287,13 @@
         <v>43</v>
       </c>
       <c r="E102" s="27" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="F102" s="27">
-        <v>4579</v>
+        <v>4186</v>
       </c>
       <c r="G102" s="27">
-        <v>6444</v>
+        <v>4578</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -8255,13 +8310,13 @@
         <v>43</v>
       </c>
       <c r="E103" s="27" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="F103" s="27">
-        <v>6445</v>
+        <v>4579</v>
       </c>
       <c r="G103" s="27">
-        <v>6822</v>
+        <v>6444</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -8278,13 +8333,13 @@
         <v>43</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="F104" s="27">
-        <v>6823</v>
+        <v>6445</v>
       </c>
       <c r="G104" s="27">
-        <v>6891</v>
+        <v>6822</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -8301,13 +8356,13 @@
         <v>43</v>
       </c>
       <c r="E105" s="27" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
       <c r="F105" s="27">
-        <v>6892</v>
+        <v>6823</v>
       </c>
       <c r="G105" s="27">
-        <v>7647</v>
+        <v>6891</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -8324,13 +8379,13 @@
         <v>43</v>
       </c>
       <c r="E106" s="27" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="F106" s="27">
-        <v>7648</v>
+        <v>6892</v>
       </c>
       <c r="G106" s="27">
-        <v>10356</v>
+        <v>7647</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -8347,36 +8402,36 @@
         <v>43</v>
       </c>
       <c r="E107" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F107" s="27">
+        <v>7648</v>
+      </c>
+      <c r="G107" s="27">
+        <v>10356</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B108" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C108" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D108" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E108" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F107" s="27">
+      <c r="F108" s="27">
         <v>10357</v>
       </c>
-      <c r="G107" s="27">
+      <c r="G108" s="27">
         <v>10839</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B108" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C108" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D108" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E108" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F108" s="27">
-        <v>1</v>
-      </c>
-      <c r="G108" s="27">
-        <v>9646</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -8393,13 +8448,13 @@
         <v>107</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F109" s="27">
         <v>1</v>
       </c>
       <c r="G109" s="27">
-        <v>341</v>
+        <v>9646</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -8416,13 +8471,13 @@
         <v>107</v>
       </c>
       <c r="E110" s="27" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F110" s="27">
-        <v>342</v>
+        <v>1</v>
       </c>
       <c r="G110" s="27">
-        <v>9377</v>
+        <v>341</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -8439,13 +8494,13 @@
         <v>107</v>
       </c>
       <c r="E111" s="27" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="F111" s="27">
         <v>342</v>
       </c>
       <c r="G111" s="27">
-        <v>2579</v>
+        <v>9377</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -8462,13 +8517,13 @@
         <v>107</v>
       </c>
       <c r="E112" s="27" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="F112" s="27">
         <v>342</v>
       </c>
       <c r="G112" s="27">
-        <v>914</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -8485,13 +8540,13 @@
         <v>107</v>
       </c>
       <c r="E113" s="27" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="F113" s="27">
-        <v>915</v>
+        <v>342</v>
       </c>
       <c r="G113" s="27">
-        <v>1490</v>
+        <v>914</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -8508,13 +8563,13 @@
         <v>107</v>
       </c>
       <c r="E114" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F114" s="27">
-        <v>1491</v>
+        <v>915</v>
       </c>
       <c r="G114" s="27">
-        <v>2579</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -8531,13 +8586,13 @@
         <v>107</v>
       </c>
       <c r="E115" s="27" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F115" s="27">
-        <v>2580</v>
+        <v>1491</v>
       </c>
       <c r="G115" s="27">
-        <v>9374</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -8554,13 +8609,13 @@
         <v>107</v>
       </c>
       <c r="E116" s="27" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="F116" s="27">
         <v>2580</v>
       </c>
       <c r="G116" s="27">
-        <v>2768</v>
+        <v>9374</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -8577,13 +8632,13 @@
         <v>107</v>
       </c>
       <c r="E117" s="27" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F117" s="27">
-        <v>2769</v>
+        <v>2580</v>
       </c>
       <c r="G117" s="27">
-        <v>3419</v>
+        <v>2768</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -8600,13 +8655,13 @@
         <v>107</v>
       </c>
       <c r="E118" s="27" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="F118" s="27">
-        <v>3420</v>
+        <v>2769</v>
       </c>
       <c r="G118" s="27">
-        <v>5312</v>
+        <v>3419</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -8623,13 +8678,13 @@
         <v>107</v>
       </c>
       <c r="E119" s="27" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="F119" s="27">
-        <v>5313</v>
+        <v>3420</v>
       </c>
       <c r="G119" s="27">
-        <v>5474</v>
+        <v>5312</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -8646,13 +8701,13 @@
         <v>107</v>
       </c>
       <c r="E120" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F120" s="27">
-        <v>5475</v>
+        <v>5313</v>
       </c>
       <c r="G120" s="27">
-        <v>6257</v>
+        <v>5474</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -8669,13 +8724,13 @@
         <v>107</v>
       </c>
       <c r="E121" s="27" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="F121" s="27">
-        <v>6258</v>
+        <v>5475</v>
       </c>
       <c r="G121" s="27">
-        <v>9374</v>
+        <v>6257</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -8692,13 +8747,13 @@
         <v>107</v>
       </c>
       <c r="E122" s="27" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F122" s="27">
         <v>6258</v>
       </c>
       <c r="G122" s="27">
-        <v>7601</v>
+        <v>9374</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -8715,13 +8770,13 @@
         <v>107</v>
       </c>
       <c r="E123" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F123" s="27">
-        <v>7602</v>
+        <v>6258</v>
       </c>
       <c r="G123" s="27">
-        <v>9374</v>
+        <v>7601</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -8738,34 +8793,36 @@
         <v>107</v>
       </c>
       <c r="E124" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F124" s="27">
+        <v>7602</v>
+      </c>
+      <c r="G124" s="27">
+        <v>9374</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B125" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C125" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D125" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E125" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F124" s="27">
+      <c r="F125" s="27">
         <v>9378</v>
       </c>
-      <c r="G124" s="27">
+      <c r="G125" s="27">
         <v>9646</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7">
-      <c r="A125" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B125" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C125" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D125"/>
-      <c r="E125" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F125" s="27">
-        <v>1</v>
-      </c>
-      <c r="G125" s="27">
-        <v>9867</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -8780,13 +8837,13 @@
       </c>
       <c r="D126"/>
       <c r="E126" s="27" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F126" s="27">
         <v>1</v>
       </c>
       <c r="G126" s="27">
-        <v>327</v>
+        <v>9867</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -8801,13 +8858,13 @@
       </c>
       <c r="D127"/>
       <c r="E127" s="27" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F127" s="27">
-        <v>328</v>
+        <v>1</v>
       </c>
       <c r="G127" s="27">
-        <v>9501</v>
+        <v>327</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -8822,13 +8879,13 @@
       </c>
       <c r="D128"/>
       <c r="E128" s="27" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="F128" s="27">
         <v>328</v>
       </c>
       <c r="G128" s="27">
-        <v>2199</v>
+        <v>9501</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -8843,13 +8900,13 @@
       </c>
       <c r="D129"/>
       <c r="E129" s="27" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="F129" s="27">
         <v>328</v>
       </c>
       <c r="G129" s="27">
-        <v>564</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -8864,13 +8921,13 @@
       </c>
       <c r="D130"/>
       <c r="E130" s="27" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="F130" s="27">
-        <v>565</v>
+        <v>328</v>
       </c>
       <c r="G130" s="27">
-        <v>1137</v>
+        <v>564</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -8885,13 +8942,13 @@
       </c>
       <c r="D131"/>
       <c r="E131" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F131" s="27">
-        <v>1138</v>
+        <v>565</v>
       </c>
       <c r="G131" s="27">
-        <v>2199</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -8906,13 +8963,13 @@
       </c>
       <c r="D132"/>
       <c r="E132" s="27" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="F132" s="27">
-        <v>2200</v>
+        <v>1138</v>
       </c>
       <c r="G132" s="27">
-        <v>2910</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -8927,13 +8984,13 @@
       </c>
       <c r="D133"/>
       <c r="E133" s="27" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="F133" s="27">
-        <v>2911</v>
+        <v>2200</v>
       </c>
       <c r="G133" s="27">
-        <v>9498</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -8948,13 +9005,13 @@
       </c>
       <c r="D134"/>
       <c r="E134" s="27" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F134" s="27">
         <v>2911</v>
       </c>
       <c r="G134" s="27">
-        <v>3630</v>
+        <v>9498</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -8969,13 +9026,13 @@
       </c>
       <c r="D135"/>
       <c r="E135" s="27" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="F135" s="27">
-        <v>3631</v>
+        <v>2911</v>
       </c>
       <c r="G135" s="27">
-        <v>5514</v>
+        <v>3630</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -8990,13 +9047,13 @@
       </c>
       <c r="D136"/>
       <c r="E136" s="27" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="F136" s="27">
-        <v>5515</v>
+        <v>3631</v>
       </c>
       <c r="G136" s="27">
-        <v>5637</v>
+        <v>5514</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -9011,13 +9068,13 @@
       </c>
       <c r="D137"/>
       <c r="E137" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F137" s="27">
-        <v>5638</v>
+        <v>5515</v>
       </c>
       <c r="G137" s="27">
-        <v>6423</v>
+        <v>5637</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -9032,13 +9089,13 @@
       </c>
       <c r="D138"/>
       <c r="E138" s="27" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="F138" s="27">
-        <v>6424</v>
+        <v>5638</v>
       </c>
       <c r="G138" s="27">
-        <v>9498</v>
+        <v>6423</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -9053,13 +9110,13 @@
       </c>
       <c r="D139"/>
       <c r="E139" s="27" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F139" s="27">
         <v>6424</v>
       </c>
       <c r="G139" s="27">
-        <v>7797</v>
+        <v>9498</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -9074,13 +9131,13 @@
       </c>
       <c r="D140"/>
       <c r="E140" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F140" s="27">
-        <v>7798</v>
+        <v>6424</v>
       </c>
       <c r="G140" s="27">
-        <v>9498</v>
+        <v>7797</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -9095,36 +9152,34 @@
       </c>
       <c r="D141"/>
       <c r="E141" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F141" s="27">
+        <v>7798</v>
+      </c>
+      <c r="G141" s="27">
+        <v>9498</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B142" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C142" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D142"/>
+      <c r="E142" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F141" s="27">
+      <c r="F142" s="27">
         <v>9502</v>
       </c>
-      <c r="G141" s="27">
+      <c r="G142" s="27">
         <v>9867</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7">
-      <c r="A142" t="s">
-        <v>54</v>
-      </c>
-      <c r="B142" t="s">
-        <v>63</v>
-      </c>
-      <c r="C142" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D142" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="E142" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F142" s="27">
-        <v>1</v>
-      </c>
-      <c r="G142" s="27">
-        <v>19199</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -9141,13 +9196,13 @@
         <v>110</v>
       </c>
       <c r="E143" s="27" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F143" s="27">
         <v>1</v>
       </c>
       <c r="G143" s="27">
-        <v>350</v>
+        <v>19199</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -9164,13 +9219,13 @@
         <v>110</v>
       </c>
       <c r="E144" s="27" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F144" s="27">
-        <v>351</v>
+        <v>1</v>
       </c>
       <c r="G144" s="27">
-        <v>18068</v>
+        <v>350</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -9187,40 +9242,40 @@
         <v>110</v>
       </c>
       <c r="E145" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F145" s="27">
+        <v>351</v>
+      </c>
+      <c r="G145" s="27">
+        <v>18068</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" t="s">
+        <v>54</v>
+      </c>
+      <c r="B146" t="s">
+        <v>63</v>
+      </c>
+      <c r="C146" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D146" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="E146" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F145" s="27">
+      <c r="F146" s="27">
         <v>18069</v>
       </c>
-      <c r="G145" s="27">
+      <c r="G146" s="27">
         <v>19199</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
-      <c r="A146" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B146" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C146" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="D146" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E146" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F146" s="27">
-        <v>1</v>
-      </c>
-      <c r="G146" s="27">
-        <v>18554</v>
-      </c>
-    </row>
     <row r="147" spans="1:7">
-      <c r="A147" s="34" t="s">
+      <c r="A147" s="32" t="s">
         <v>84</v>
       </c>
       <c r="B147" s="32" t="s">
@@ -9233,13 +9288,13 @@
         <v>111</v>
       </c>
       <c r="E147" s="27" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F147" s="27">
         <v>1</v>
       </c>
       <c r="G147" s="27">
-        <v>199</v>
+        <v>18554</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -9256,13 +9311,13 @@
         <v>111</v>
       </c>
       <c r="E148" s="27" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F148" s="27">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="G148" s="27">
-        <v>17905</v>
+        <v>199</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -9279,34 +9334,36 @@
         <v>111</v>
       </c>
       <c r="E149" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F149" s="27">
+        <v>200</v>
+      </c>
+      <c r="G149" s="27">
+        <v>17905</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B150" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C150" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D150" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E150" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F149" s="27">
+      <c r="F150" s="27">
         <v>17906</v>
       </c>
-      <c r="G149" s="27">
+      <c r="G150" s="27">
         <v>18554</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7">
-      <c r="A150" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B150" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C150" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D150" s="27"/>
-      <c r="E150" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F150" s="27">
-        <v>1</v>
-      </c>
-      <c r="G150" s="27">
-        <v>12573</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -9321,13 +9378,13 @@
       </c>
       <c r="D151" s="27"/>
       <c r="E151" s="27" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F151" s="27">
         <v>1</v>
       </c>
       <c r="G151" s="27">
-        <v>385</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -9342,13 +9399,13 @@
       </c>
       <c r="D152" s="27"/>
       <c r="E152" s="27" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F152" s="27">
-        <v>386</v>
+        <v>1</v>
       </c>
       <c r="G152" s="27">
-        <v>12352</v>
+        <v>385</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -9363,13 +9420,13 @@
       </c>
       <c r="D153" s="27"/>
       <c r="E153" s="27" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="F153" s="27">
         <v>386</v>
       </c>
       <c r="G153" s="27">
-        <v>3583</v>
+        <v>12352</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -9384,13 +9441,13 @@
       </c>
       <c r="D154" s="27"/>
       <c r="E154" s="27" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="F154" s="27">
         <v>386</v>
       </c>
       <c r="G154" s="27">
-        <v>889</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -9405,13 +9462,13 @@
       </c>
       <c r="D155" s="27"/>
       <c r="E155" s="27" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="F155" s="27">
-        <v>890</v>
+        <v>386</v>
       </c>
       <c r="G155" s="27">
-        <v>1195</v>
+        <v>889</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -9426,13 +9483,13 @@
       </c>
       <c r="D156" s="27"/>
       <c r="E156" s="27" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="F156" s="27">
-        <v>1196</v>
+        <v>890</v>
       </c>
       <c r="G156" s="27">
-        <v>1876</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -9447,13 +9504,13 @@
       </c>
       <c r="D157" s="27"/>
       <c r="E157" s="27" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="F157" s="27">
-        <v>1877</v>
+        <v>1196</v>
       </c>
       <c r="G157" s="27">
-        <v>2461</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -9468,13 +9525,13 @@
       </c>
       <c r="D158" s="27"/>
       <c r="E158" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F158" s="27">
-        <v>2462</v>
+        <v>1877</v>
       </c>
       <c r="G158" s="27">
-        <v>3583</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -9489,13 +9546,13 @@
       </c>
       <c r="D159" s="27"/>
       <c r="E159" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F159" s="27">
-        <v>3584</v>
+        <v>2462</v>
       </c>
       <c r="G159" s="27">
-        <v>3793</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -9510,13 +9567,13 @@
       </c>
       <c r="D160" s="27"/>
       <c r="E160" s="27" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="F160" s="27">
-        <v>3794</v>
+        <v>3584</v>
       </c>
       <c r="G160" s="27">
-        <v>7471</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -9531,13 +9588,13 @@
       </c>
       <c r="D161" s="27"/>
       <c r="E161" s="27" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="F161" s="27">
-        <v>7472</v>
+        <v>3794</v>
       </c>
       <c r="G161" s="27">
-        <v>7663</v>
+        <v>7471</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -9552,13 +9609,13 @@
       </c>
       <c r="D162" s="27"/>
       <c r="E162" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F162" s="27">
-        <v>7664</v>
+        <v>7472</v>
       </c>
       <c r="G162" s="27">
-        <v>8704</v>
+        <v>7663</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -9573,13 +9630,13 @@
       </c>
       <c r="D163" s="27"/>
       <c r="E163" s="27" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="F163" s="27">
-        <v>8705</v>
+        <v>7664</v>
       </c>
       <c r="G163" s="27">
-        <v>12349</v>
+        <v>8704</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -9594,13 +9651,13 @@
       </c>
       <c r="D164" s="27"/>
       <c r="E164" s="27" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F164" s="27">
         <v>8705</v>
       </c>
       <c r="G164" s="27">
-        <v>10192</v>
+        <v>12349</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -9615,13 +9672,13 @@
       </c>
       <c r="D165" s="27"/>
       <c r="E165" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F165" s="27">
-        <v>10193</v>
+        <v>8705</v>
       </c>
       <c r="G165" s="27">
-        <v>12349</v>
+        <v>10192</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -9636,34 +9693,34 @@
       </c>
       <c r="D166" s="27"/>
       <c r="E166" s="27" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F166" s="27">
-        <v>12360</v>
+        <v>10193</v>
       </c>
       <c r="G166" s="27">
-        <v>12573</v>
+        <v>12349</v>
       </c>
     </row>
     <row r="167" spans="1:7">
-      <c r="A167" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B167" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C167" s="27" t="s">
-        <v>57</v>
+      <c r="A167" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B167" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C167" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D167" s="27"/>
       <c r="E167" s="27" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="F167" s="27">
-        <v>1</v>
+        <v>12360</v>
       </c>
       <c r="G167" s="27">
-        <v>10053</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -9678,7 +9735,7 @@
       </c>
       <c r="D168" s="27"/>
       <c r="E168" s="27" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F168" s="27">
         <v>1</v>
@@ -9699,13 +9756,13 @@
       </c>
       <c r="D169" s="27"/>
       <c r="E169" s="27" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="F169" s="27">
         <v>1</v>
       </c>
       <c r="G169" s="27">
-        <v>2358</v>
+        <v>10053</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -9720,13 +9777,13 @@
       </c>
       <c r="D170" s="27"/>
       <c r="E170" s="27" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="F170" s="27">
         <v>1</v>
       </c>
       <c r="G170" s="27">
-        <v>345</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -9741,13 +9798,13 @@
       </c>
       <c r="D171" s="27"/>
       <c r="E171" s="27" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="F171" s="27">
-        <v>346</v>
+        <v>1</v>
       </c>
       <c r="G171" s="27">
-        <v>852</v>
+        <v>345</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -9762,10 +9819,10 @@
       </c>
       <c r="D172" s="27"/>
       <c r="E172" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F172" s="27">
-        <v>655</v>
+        <v>346</v>
       </c>
       <c r="G172" s="27">
         <v>852</v>
@@ -9783,13 +9840,13 @@
       </c>
       <c r="D173" s="27"/>
       <c r="E173" s="27" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="F173" s="27">
-        <v>853</v>
+        <v>655</v>
       </c>
       <c r="G173" s="27">
-        <v>2358</v>
+        <v>852</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -9804,13 +9861,13 @@
       </c>
       <c r="D174" s="27"/>
       <c r="E174" s="27" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="F174" s="27">
-        <v>2359</v>
+        <v>853</v>
       </c>
       <c r="G174" s="27">
-        <v>10050</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -9825,13 +9882,13 @@
       </c>
       <c r="D175" s="27"/>
       <c r="E175" s="27" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
       <c r="F175" s="27">
         <v>2359</v>
       </c>
       <c r="G175" s="27">
-        <v>3390</v>
+        <v>10050</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -9846,13 +9903,13 @@
       </c>
       <c r="D176" s="27"/>
       <c r="E176" s="27" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="F176" s="27">
-        <v>3391</v>
+        <v>2359</v>
       </c>
       <c r="G176" s="27">
-        <v>3978</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -9867,13 +9924,13 @@
       </c>
       <c r="D177" s="27"/>
       <c r="E177" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F177" s="27">
-        <v>3979</v>
+        <v>3391</v>
       </c>
       <c r="G177" s="27">
-        <v>4431</v>
+        <v>3978</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -9888,13 +9945,13 @@
       </c>
       <c r="D178" s="27"/>
       <c r="E178" s="27" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="F178" s="27">
-        <v>4432</v>
+        <v>3979</v>
       </c>
       <c r="G178" s="27">
-        <v>6303</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -9909,13 +9966,13 @@
       </c>
       <c r="D179" s="27"/>
       <c r="E179" s="27" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="F179" s="27">
-        <v>6304</v>
+        <v>4432</v>
       </c>
       <c r="G179" s="27">
-        <v>6687</v>
+        <v>6303</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -9930,13 +9987,13 @@
       </c>
       <c r="D180" s="27"/>
       <c r="E180" s="27" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="F180" s="27">
-        <v>6688</v>
+        <v>6304</v>
       </c>
       <c r="G180" s="27">
-        <v>6762</v>
+        <v>6687</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -9951,13 +10008,13 @@
       </c>
       <c r="D181" s="27"/>
       <c r="E181" s="27" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
       <c r="F181" s="27">
-        <v>6763</v>
+        <v>6688</v>
       </c>
       <c r="G181" s="27">
-        <v>7557</v>
+        <v>6762</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -9972,45 +10029,43 @@
       </c>
       <c r="D182" s="27"/>
       <c r="E182" s="27" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="F182" s="27">
-        <v>7558</v>
+        <v>6763</v>
       </c>
       <c r="G182" s="27">
-        <v>10050</v>
-      </c>
-      <c r="H182" s="25"/>
+        <v>7557</v>
+      </c>
     </row>
     <row r="183" spans="1:8">
       <c r="A183" s="27" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
       <c r="B183" s="27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C183" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D183" s="27" t="s">
-        <v>112</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D183" s="27"/>
       <c r="E183" s="27" t="s">
         <v>10</v>
       </c>
       <c r="F183" s="27">
-        <v>105</v>
+        <v>7558</v>
       </c>
       <c r="G183" s="27">
-        <v>2849</v>
-      </c>
+        <v>10050</v>
+      </c>
+      <c r="H183" s="25"/>
     </row>
     <row r="184" spans="1:8">
-      <c r="A184" t="s">
-        <v>113</v>
+      <c r="A184" s="27" t="s">
+        <v>108</v>
       </c>
       <c r="B184" s="27" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="C184" s="27" t="s">
         <v>109</v>
@@ -10019,21 +10074,21 @@
         <v>112</v>
       </c>
       <c r="E184" s="27" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F184" s="27">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G184" s="27">
-        <v>2543</v>
+        <v>2849</v>
       </c>
     </row>
     <row r="185" spans="1:8">
-      <c r="A185" s="27" t="s">
-        <v>108</v>
+      <c r="A185" t="s">
+        <v>113</v>
       </c>
       <c r="B185" s="27" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="C185" s="27" t="s">
         <v>109</v>
@@ -10042,67 +10097,67 @@
         <v>112</v>
       </c>
       <c r="E185" s="27" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="F185" s="27">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="G185" s="27">
-        <v>2849</v>
+        <v>2543</v>
       </c>
     </row>
     <row r="186" spans="1:8">
-      <c r="A186" t="s">
-        <v>113</v>
+      <c r="A186" s="27" t="s">
+        <v>108</v>
       </c>
       <c r="B186" s="27" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="C186" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="27" t="s">
         <v>112</v>
       </c>
       <c r="E186" s="27" t="s">
         <v>70</v>
       </c>
       <c r="F186" s="27">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G186" s="27">
-        <v>2543</v>
+        <v>2849</v>
       </c>
     </row>
     <row r="187" spans="1:8">
       <c r="A187" t="s">
-        <v>108</v>
-      </c>
-      <c r="B187" t="s">
-        <v>65</v>
-      </c>
-      <c r="C187" t="s">
+        <v>113</v>
+      </c>
+      <c r="B187" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C187" s="27" t="s">
         <v>109</v>
       </c>
       <c r="D187" t="s">
         <v>112</v>
       </c>
-      <c r="E187" t="s">
-        <v>83</v>
-      </c>
-      <c r="F187">
-        <v>1</v>
-      </c>
-      <c r="G187">
-        <v>3114</v>
+      <c r="E187" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F187" s="27">
+        <v>117</v>
+      </c>
+      <c r="G187" s="27">
+        <v>2543</v>
       </c>
     </row>
     <row r="188" spans="1:8">
       <c r="A188" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B188" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="C188" t="s">
         <v>109</v>
@@ -10117,17 +10172,35 @@
         <v>1</v>
       </c>
       <c r="G188">
+        <v>3114</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8">
+      <c r="A189" t="s">
+        <v>113</v>
+      </c>
+      <c r="B189" t="s">
+        <v>114</v>
+      </c>
+      <c r="C189" t="s">
+        <v>109</v>
+      </c>
+      <c r="D189" t="s">
+        <v>112</v>
+      </c>
+      <c r="E189" t="s">
+        <v>83</v>
+      </c>
+      <c r="F189">
+        <v>1</v>
+      </c>
+      <c r="G189">
         <v>2824</v>
       </c>
-    </row>
-    <row r="224" spans="2:3">
-      <c r="B224" s="1"/>
-      <c r="C224" s="5"/>
     </row>
     <row r="225" spans="2:4">
       <c r="B225" s="1"/>
       <c r="C225" s="5"/>
-      <c r="D225" s="5"/>
     </row>
     <row r="226" spans="2:4">
       <c r="B226" s="1"/>
@@ -10241,16 +10314,16 @@
     </row>
     <row r="248" spans="2:4">
       <c r="B248" s="1"/>
+      <c r="C248" s="5"/>
       <c r="D248" s="5"/>
     </row>
     <row r="249" spans="2:4">
       <c r="B249" s="1"/>
-      <c r="C249" s="5"/>
+      <c r="D249" s="5"/>
     </row>
     <row r="250" spans="2:4">
       <c r="B250" s="1"/>
       <c r="C250" s="5"/>
-      <c r="D250" s="5"/>
     </row>
     <row r="251" spans="2:4">
       <c r="B251" s="1"/>
@@ -10278,19 +10351,21 @@
       <c r="D255" s="5"/>
     </row>
     <row r="256" spans="2:4">
+      <c r="B256" s="1"/>
+      <c r="C256" s="5"/>
       <c r="D256" s="5"/>
     </row>
-    <row r="938" spans="5:5">
-      <c r="E938" s="1"/>
-    </row>
-    <row r="1074" spans="2:2">
-      <c r="B1074" s="1"/>
+    <row r="257" spans="4:4">
+      <c r="D257" s="5"/>
+    </row>
+    <row r="939" spans="5:5">
+      <c r="E939" s="1"/>
     </row>
     <row r="1075" spans="2:2">
       <c r="B1075" s="1"/>
     </row>
-    <row r="1200" spans="2:2">
-      <c r="B1200" s="1"/>
+    <row r="1076" spans="2:2">
+      <c r="B1076" s="1"/>
     </row>
     <row r="1201" spans="2:2">
       <c r="B1201" s="1"/>
@@ -10307,9 +10382,8 @@
     <row r="1205" spans="2:2">
       <c r="B1205" s="1"/>
     </row>
-    <row r="1250" spans="2:6">
-      <c r="E1250" s="1"/>
-      <c r="F1250" s="1"/>
+    <row r="1206" spans="2:2">
+      <c r="B1206" s="1"/>
     </row>
     <row r="1251" spans="2:6">
       <c r="E1251" s="1"/>
@@ -10319,8 +10393,9 @@
       <c r="E1252" s="1"/>
       <c r="F1252" s="1"/>
     </row>
-    <row r="1254" spans="2:6">
-      <c r="B1254" s="1"/>
+    <row r="1253" spans="2:6">
+      <c r="E1253" s="1"/>
+      <c r="F1253" s="1"/>
     </row>
     <row r="1255" spans="2:6">
       <c r="B1255" s="1"/>
@@ -10334,8 +10409,8 @@
     <row r="1258" spans="2:6">
       <c r="B1258" s="1"/>
     </row>
-    <row r="1277" spans="2:2">
-      <c r="B1277" s="1"/>
+    <row r="1259" spans="2:6">
+      <c r="B1259" s="1"/>
     </row>
     <row r="1278" spans="2:2">
       <c r="B1278" s="1"/>
@@ -10355,8 +10430,8 @@
     <row r="1283" spans="2:2">
       <c r="B1283" s="1"/>
     </row>
-    <row r="1285" spans="2:2">
-      <c r="B1285" s="1"/>
+    <row r="1284" spans="2:2">
+      <c r="B1284" s="1"/>
     </row>
     <row r="1286" spans="2:2">
       <c r="B1286" s="1"/>
@@ -10373,8 +10448,8 @@
     <row r="1290" spans="2:2">
       <c r="B1290" s="1"/>
     </row>
-    <row r="1342" spans="2:2">
-      <c r="B1342" s="1"/>
+    <row r="1291" spans="2:2">
+      <c r="B1291" s="1"/>
     </row>
     <row r="1343" spans="2:2">
       <c r="B1343" s="1"/>
@@ -10385,8 +10460,8 @@
     <row r="1345" spans="2:2">
       <c r="B1345" s="1"/>
     </row>
-    <row r="1347" spans="2:2">
-      <c r="B1347" s="1"/>
+    <row r="1346" spans="2:2">
+      <c r="B1346" s="1"/>
     </row>
     <row r="1348" spans="2:2">
       <c r="B1348" s="1"/>
@@ -10397,8 +10472,8 @@
     <row r="1350" spans="2:2">
       <c r="B1350" s="1"/>
     </row>
-    <row r="1385" spans="2:2">
-      <c r="B1385" s="1"/>
+    <row r="1351" spans="2:2">
+      <c r="B1351" s="1"/>
     </row>
     <row r="1386" spans="2:2">
       <c r="B1386" s="1"/>
@@ -10415,18 +10490,15 @@
     <row r="1390" spans="2:2">
       <c r="B1390" s="1"/>
     </row>
-    <row r="1432" spans="3:6">
-      <c r="E1432" s="1"/>
-      <c r="F1432" s="1"/>
+    <row r="1391" spans="2:2">
+      <c r="B1391" s="1"/>
     </row>
     <row r="1433" spans="3:6">
-      <c r="C1433" s="6"/>
       <c r="E1433" s="1"/>
       <c r="F1433" s="1"/>
     </row>
     <row r="1434" spans="3:6">
       <c r="C1434" s="6"/>
-      <c r="D1434" s="6"/>
       <c r="E1434" s="1"/>
       <c r="F1434" s="1"/>
     </row>
@@ -10437,12 +10509,15 @@
       <c r="F1435" s="1"/>
     </row>
     <row r="1436" spans="3:6">
+      <c r="C1436" s="6"/>
       <c r="D1436" s="6"/>
       <c r="E1436" s="1"/>
       <c r="F1436" s="1"/>
     </row>
-    <row r="1499" spans="2:2">
-      <c r="B1499" s="1"/>
+    <row r="1437" spans="3:6">
+      <c r="D1437" s="6"/>
+      <c r="E1437" s="1"/>
+      <c r="F1437" s="1"/>
     </row>
     <row r="1500" spans="2:2">
       <c r="B1500" s="1"/>
@@ -10452,6 +10527,9 @@
     </row>
     <row r="1502" spans="2:2">
       <c r="B1502" s="1"/>
+    </row>
+    <row r="1503" spans="2:2">
+      <c r="B1503" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:G1456">

</xml_diff>